<commit_message>
Excel r2 colors fixed
</commit_message>
<xml_diff>
--- a/TFG_Results/Transformer_results/Transformer_metrics.xlsx
+++ b/TFG_Results/Transformer_results/Transformer_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\OneDrive\Escritorio\TFG_TST\TFG_Results\Transformer_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C37E39-CB95-4DFF-8817-B88B780F2963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4D7186-193A-4206-B350-A01F348A924C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2610" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Folder</t>
   </si>
@@ -148,13 +148,33 @@
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +191,31 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -249,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -260,6 +305,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,845 +630,850 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
+    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>-21.032771</v>
-      </c>
-      <c r="C2">
-        <v>-36.011092400000003</v>
-      </c>
-      <c r="D2">
-        <v>-15.533721699999999</v>
-      </c>
-      <c r="E2">
-        <v>-20.932425800000001</v>
-      </c>
-      <c r="F2">
-        <v>-20.5435844</v>
-      </c>
-      <c r="G2">
-        <v>-22.3636421</v>
-      </c>
-      <c r="H2" s="3">
-        <f>AVERAGE(B2:G2)</f>
-        <v>-22.736206233333334</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>-20.406924400000001</v>
+        <v>-21.032771</v>
       </c>
       <c r="C3">
-        <v>-41.049903899999997</v>
+        <v>-36.011092400000003</v>
       </c>
       <c r="D3">
-        <v>-24.157681199999999</v>
+        <v>-15.533721699999999</v>
       </c>
       <c r="E3">
-        <v>-19.944791500000001</v>
+        <v>-20.932425800000001</v>
       </c>
       <c r="F3">
-        <v>-19.389690699999999</v>
+        <v>-20.5435844</v>
       </c>
       <c r="G3">
-        <v>-18.658907200000002</v>
+        <v>-22.3636421</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H31" si="0">AVERAGE(B3:G3)</f>
-        <v>-23.934649816666667</v>
+        <f>AVERAGE(B3:G3)</f>
+        <v>-22.736206233333334</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>-19.570627399999999</v>
+        <v>-20.406924400000001</v>
       </c>
       <c r="C4">
-        <v>-42.8415052</v>
+        <v>-41.049903899999997</v>
       </c>
       <c r="D4">
-        <v>-13.427972199999999</v>
+        <v>-24.157681199999999</v>
       </c>
       <c r="E4">
-        <v>-14.385999</v>
+        <v>-19.944791500000001</v>
       </c>
       <c r="F4">
-        <v>-24.658665500000001</v>
+        <v>-19.389690699999999</v>
       </c>
       <c r="G4">
-        <v>-19.191879</v>
+        <v>-18.658907200000002</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>-22.346108049999998</v>
+        <f t="shared" ref="H4:H32" si="0">AVERAGE(B4:G4)</f>
+        <v>-23.934649816666667</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>-17.294701199999999</v>
+        <v>-19.570627399999999</v>
       </c>
       <c r="C5">
-        <v>-30.4916464</v>
+        <v>-42.8415052</v>
       </c>
       <c r="D5">
-        <v>-12.6093098</v>
+        <v>-13.427972199999999</v>
       </c>
       <c r="E5">
-        <v>-9.8376903999999996</v>
+        <v>-14.385999</v>
       </c>
       <c r="F5">
-        <v>-10.601813699999999</v>
+        <v>-24.658665500000001</v>
       </c>
       <c r="G5">
-        <v>-14.606989</v>
+        <v>-19.191879</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>-15.90702508333333</v>
+        <v>-22.346108049999998</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>-17.2872588</v>
+        <v>-17.294701199999999</v>
       </c>
       <c r="C6">
-        <v>-36.854616399999998</v>
+        <v>-30.4916464</v>
       </c>
       <c r="D6">
-        <v>-11.5675398</v>
+        <v>-12.6093098</v>
       </c>
       <c r="E6">
-        <v>-12.2167098</v>
+        <v>-9.8376903999999996</v>
       </c>
       <c r="F6">
-        <v>-15.1419671</v>
+        <v>-10.601813699999999</v>
       </c>
       <c r="G6">
-        <v>-13.018887899999999</v>
+        <v>-14.606989</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>-17.681163300000001</v>
+        <v>-15.90702508333333</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>-20.911200900000001</v>
+        <v>-17.2872588</v>
       </c>
       <c r="C7">
-        <v>-41.588087700000003</v>
+        <v>-36.854616399999998</v>
       </c>
       <c r="D7">
-        <v>-14.3505067</v>
+        <v>-11.5675398</v>
       </c>
       <c r="E7">
-        <v>-18.6842568</v>
+        <v>-12.2167098</v>
       </c>
       <c r="F7">
-        <v>-15.477086999999999</v>
+        <v>-15.1419671</v>
       </c>
       <c r="G7">
-        <v>-21.170314000000001</v>
+        <v>-13.018887899999999</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>-22.030242183333332</v>
+        <v>-17.681163300000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>-14.4346215</v>
+        <v>-20.911200900000001</v>
       </c>
       <c r="C8">
-        <v>-36.946788300000001</v>
+        <v>-41.588087700000003</v>
       </c>
       <c r="D8">
-        <v>-11.6185954</v>
+        <v>-14.3505067</v>
       </c>
       <c r="E8">
-        <v>-10.512088500000001</v>
+        <v>-18.6842568</v>
       </c>
       <c r="F8">
-        <v>-21.2859129</v>
+        <v>-15.477086999999999</v>
       </c>
       <c r="G8">
-        <v>-12.835842599999999</v>
+        <v>-21.170314000000001</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
-        <v>-17.938974866666669</v>
+        <v>-22.030242183333332</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>-18.2175999</v>
+        <v>-14.4346215</v>
       </c>
       <c r="C9">
-        <v>-31.984705200000001</v>
+        <v>-36.946788300000001</v>
       </c>
       <c r="D9">
-        <v>-13.4595447</v>
+        <v>-11.6185954</v>
       </c>
       <c r="E9">
-        <v>-14.109465500000001</v>
+        <v>-10.512088500000001</v>
       </c>
       <c r="F9">
-        <v>-19.196473399999999</v>
+        <v>-21.2859129</v>
       </c>
       <c r="G9">
-        <v>-16.701698100000002</v>
+        <v>-12.835842599999999</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>-18.94491446666667</v>
+        <v>-17.938974866666669</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>-17.250018699999998</v>
+        <v>-18.2175999</v>
       </c>
       <c r="C10">
-        <v>-31.888963799999999</v>
+        <v>-31.984705200000001</v>
       </c>
       <c r="D10">
-        <v>-14.0132931</v>
+        <v>-13.4595447</v>
       </c>
       <c r="E10">
-        <v>-14.982514200000001</v>
+        <v>-14.109465500000001</v>
       </c>
       <c r="F10">
-        <v>-12.2655283</v>
+        <v>-19.196473399999999</v>
       </c>
       <c r="G10">
-        <v>-18.328409300000001</v>
+        <v>-16.701698100000002</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>-18.121454566666667</v>
+        <v>-18.94491446666667</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>-19.5548067</v>
+        <v>-17.250018699999998</v>
       </c>
       <c r="C11">
-        <v>-25.028890799999999</v>
+        <v>-31.888963799999999</v>
       </c>
       <c r="D11">
-        <v>-13.334423900000001</v>
+        <v>-14.0132931</v>
       </c>
       <c r="E11">
-        <v>-14.161092699999999</v>
+        <v>-14.982514200000001</v>
       </c>
       <c r="F11">
-        <v>-22.432455399999998</v>
+        <v>-12.2655283</v>
       </c>
       <c r="G11">
-        <v>-16.625015600000001</v>
+        <v>-18.328409300000001</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>-18.52278085</v>
+        <v>-18.121454566666667</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>-15.7261474</v>
+        <v>-19.5548067</v>
       </c>
       <c r="C12">
-        <v>-27.276750199999999</v>
+        <v>-25.028890799999999</v>
       </c>
       <c r="D12">
-        <v>-13.1792315</v>
+        <v>-13.334423900000001</v>
       </c>
       <c r="E12">
-        <v>-11.275166199999999</v>
+        <v>-14.161092699999999</v>
       </c>
       <c r="F12">
-        <v>-16.593104499999999</v>
+        <v>-22.432455399999998</v>
       </c>
       <c r="G12">
-        <v>-15.2160967</v>
+        <v>-16.625015600000001</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="0"/>
-        <v>-16.544416083333331</v>
+        <v>-18.52278085</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>-21.9155008</v>
+        <v>-15.7261474</v>
       </c>
       <c r="C13">
-        <v>-34.797186600000003</v>
+        <v>-27.276750199999999</v>
       </c>
       <c r="D13">
-        <v>-14.1095326</v>
+        <v>-13.1792315</v>
       </c>
       <c r="E13">
-        <v>-13.4932493</v>
+        <v>-11.275166199999999</v>
       </c>
       <c r="F13">
-        <v>-17.295736099999999</v>
+        <v>-16.593104499999999</v>
       </c>
       <c r="G13">
-        <v>-15.225873399999999</v>
+        <v>-15.2160967</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="0"/>
-        <v>-19.472846466666667</v>
+        <v>-16.544416083333331</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>-22.651688400000001</v>
+        <v>-21.9155008</v>
       </c>
       <c r="C14">
-        <v>-25.245136800000001</v>
+        <v>-34.797186600000003</v>
       </c>
       <c r="D14">
-        <v>-14.0649937</v>
+        <v>-14.1095326</v>
       </c>
       <c r="E14">
-        <v>-14.3514952</v>
+        <v>-13.4932493</v>
       </c>
       <c r="F14">
-        <v>-12.0631833</v>
+        <v>-17.295736099999999</v>
       </c>
       <c r="G14">
-        <v>-16.922112500000001</v>
+        <v>-15.225873399999999</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="0"/>
-        <v>-17.549768316666668</v>
+        <v>-19.472846466666667</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>-19.461395199999998</v>
+        <v>-22.651688400000001</v>
       </c>
       <c r="C15">
-        <v>-23.069005499999999</v>
+        <v>-25.245136800000001</v>
       </c>
       <c r="D15">
-        <v>-14.026277800000001</v>
+        <v>-14.0649937</v>
       </c>
       <c r="E15">
-        <v>-19.150310300000001</v>
+        <v>-14.3514952</v>
       </c>
       <c r="F15">
-        <v>-12.1621197</v>
+        <v>-12.0631833</v>
       </c>
       <c r="G15">
-        <v>-20.3138197</v>
+        <v>-16.922112500000001</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="0"/>
-        <v>-18.030488033333334</v>
+        <v>-17.549768316666668</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>-20.476213999999999</v>
+        <v>-19.461395199999998</v>
       </c>
       <c r="C16">
-        <v>-30.296253199999999</v>
+        <v>-23.069005499999999</v>
       </c>
       <c r="D16">
-        <v>-14.2529889</v>
+        <v>-14.026277800000001</v>
       </c>
       <c r="E16">
-        <v>-15.438332000000001</v>
+        <v>-19.150310300000001</v>
       </c>
       <c r="F16">
-        <v>-23.2839563</v>
+        <v>-12.1621197</v>
       </c>
       <c r="G16">
-        <v>-17.853883700000001</v>
+        <v>-20.3138197</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="0"/>
-        <v>-20.266938016666668</v>
+        <v>-18.030488033333334</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>-19.754861399999999</v>
+        <v>-20.476213999999999</v>
       </c>
       <c r="C17">
-        <v>-37.6378755</v>
+        <v>-30.296253199999999</v>
       </c>
       <c r="D17">
-        <v>-13.064559300000001</v>
+        <v>-14.2529889</v>
       </c>
       <c r="E17">
-        <v>-8.3234320999999998</v>
+        <v>-15.438332000000001</v>
       </c>
       <c r="F17">
-        <v>-12.232351700000001</v>
+        <v>-23.2839563</v>
       </c>
       <c r="G17">
-        <v>-16.7883104</v>
+        <v>-17.853883700000001</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="0"/>
-        <v>-17.966898400000002</v>
+        <v>-20.266938016666668</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>-18.992035900000001</v>
+        <v>-19.754861399999999</v>
       </c>
       <c r="C18">
-        <v>-36.809140499999998</v>
+        <v>-37.6378755</v>
       </c>
       <c r="D18">
-        <v>-12.5907407</v>
+        <v>-13.064559300000001</v>
       </c>
       <c r="E18">
-        <v>-10.951613699999999</v>
+        <v>-8.3234320999999998</v>
       </c>
       <c r="F18">
-        <v>-12.355860099999999</v>
+        <v>-12.232351700000001</v>
       </c>
       <c r="G18">
-        <v>-15.5308291</v>
+        <v>-16.7883104</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="0"/>
-        <v>-17.871703333333333</v>
+        <v>-17.966898400000002</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>-21.5816029</v>
+        <v>-18.992035900000001</v>
       </c>
       <c r="C19">
-        <v>-19.955765599999999</v>
+        <v>-36.809140499999998</v>
       </c>
       <c r="D19">
-        <v>-13.933817700000001</v>
+        <v>-12.5907407</v>
       </c>
       <c r="E19">
-        <v>-10.044253100000001</v>
+        <v>-10.951613699999999</v>
       </c>
       <c r="F19">
-        <v>-8.7419446999999995</v>
+        <v>-12.355860099999999</v>
       </c>
       <c r="G19">
-        <v>-18.710442499999999</v>
+        <v>-15.5308291</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="0"/>
-        <v>-15.494637750000001</v>
+        <v>-17.871703333333333</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>-20.989706399999999</v>
+        <v>-21.5816029</v>
       </c>
       <c r="C20">
-        <v>-43.193805500000003</v>
+        <v>-19.955765599999999</v>
       </c>
       <c r="D20">
-        <v>-14.5751621</v>
+        <v>-13.933817700000001</v>
       </c>
       <c r="E20">
-        <v>-13.536150599999999</v>
+        <v>-10.044253100000001</v>
       </c>
       <c r="F20">
-        <v>-21.043924100000002</v>
+        <v>-8.7419446999999995</v>
       </c>
       <c r="G20">
-        <v>-19.5807295</v>
+        <v>-18.710442499999999</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="0"/>
-        <v>-22.153246366666664</v>
+        <v>-15.494637750000001</v>
       </c>
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>-17.071313199999999</v>
+        <v>-20.989706399999999</v>
       </c>
       <c r="C21">
-        <v>-31.956562300000002</v>
+        <v>-43.193805500000003</v>
       </c>
       <c r="D21">
-        <v>-13.4470721</v>
+        <v>-14.5751621</v>
       </c>
       <c r="E21">
-        <v>-13.079902499999999</v>
+        <v>-13.536150599999999</v>
       </c>
       <c r="F21">
-        <v>-13.011406300000001</v>
+        <v>-21.043924100000002</v>
       </c>
       <c r="G21">
-        <v>-14.4059046</v>
+        <v>-19.5807295</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="0"/>
-        <v>-17.162026833333332</v>
+        <v>-22.153246366666664</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>-24.135540899999999</v>
+        <v>-17.071313199999999</v>
       </c>
       <c r="C22">
-        <v>-23.9283909</v>
+        <v>-31.956562300000002</v>
       </c>
       <c r="D22">
-        <v>-15.604567299999999</v>
+        <v>-13.4470721</v>
       </c>
       <c r="E22">
-        <v>-21.3973215</v>
+        <v>-13.079902499999999</v>
       </c>
       <c r="F22">
-        <v>-11.8342948</v>
+        <v>-13.011406300000001</v>
       </c>
       <c r="G22">
-        <v>-23.898673800000001</v>
+        <v>-14.4059046</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="0"/>
-        <v>-20.13313153333333</v>
+        <v>-17.162026833333332</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>-20.433776999999999</v>
+        <v>-24.135540899999999</v>
       </c>
       <c r="C23">
-        <v>-38.852964299999996</v>
+        <v>-23.9283909</v>
       </c>
       <c r="D23">
-        <v>-13.1445095</v>
+        <v>-15.604567299999999</v>
       </c>
       <c r="E23">
-        <v>-12.014249299999999</v>
+        <v>-21.3973215</v>
       </c>
       <c r="F23">
-        <v>-22.7017396</v>
+        <v>-11.8342948</v>
       </c>
       <c r="G23">
-        <v>-18.745516299999998</v>
+        <v>-23.898673800000001</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" si="0"/>
-        <v>-20.982125999999997</v>
+        <v>-20.13313153333333</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>-20.025093699999999</v>
+        <v>-20.433776999999999</v>
       </c>
       <c r="C24">
-        <v>-25.214934</v>
+        <v>-38.852964299999996</v>
       </c>
       <c r="D24">
-        <v>-14.6063376</v>
+        <v>-13.1445095</v>
       </c>
       <c r="E24">
-        <v>-19.2521974</v>
+        <v>-12.014249299999999</v>
       </c>
       <c r="F24">
-        <v>-9.6140931999999992</v>
+        <v>-22.7017396</v>
       </c>
       <c r="G24">
-        <v>-16.289753099999999</v>
+        <v>-18.745516299999998</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="0"/>
-        <v>-17.500401499999999</v>
+        <v>-20.982125999999997</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>-20.381800500000001</v>
+        <v>-20.025093699999999</v>
       </c>
       <c r="C25">
-        <v>-23.336405299999999</v>
+        <v>-25.214934</v>
       </c>
       <c r="D25">
-        <v>-14.7327732</v>
+        <v>-14.6063376</v>
       </c>
       <c r="E25">
-        <v>-13.7929718</v>
+        <v>-19.2521974</v>
       </c>
       <c r="F25">
-        <v>-25.966559100000001</v>
+        <v>-9.6140931999999992</v>
       </c>
       <c r="G25">
-        <v>-17.677706400000002</v>
+        <v>-16.289753099999999</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="0"/>
-        <v>-19.31470271666667</v>
+        <v>-17.500401499999999</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>-21.835591999999998</v>
+        <v>-20.381800500000001</v>
       </c>
       <c r="C26">
-        <v>-19.674721999999999</v>
+        <v>-23.336405299999999</v>
       </c>
       <c r="D26">
-        <v>-13.203061</v>
+        <v>-14.7327732</v>
       </c>
       <c r="E26">
-        <v>-15.570838999999999</v>
+        <v>-13.7929718</v>
       </c>
       <c r="F26">
-        <v>-4.9544290000000002</v>
+        <v>-25.966559100000001</v>
       </c>
       <c r="G26">
-        <v>-18.15232</v>
+        <v>-17.677706400000002</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="0"/>
-        <v>-15.565160499999999</v>
+        <v>-19.31470271666667</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>-17.024256900000001</v>
+        <v>-21.835591999999998</v>
       </c>
       <c r="C27">
-        <v>-35.764348699999999</v>
+        <v>-19.674721999999999</v>
       </c>
       <c r="D27">
-        <v>-12.6528718</v>
+        <v>-13.203061</v>
       </c>
       <c r="E27">
-        <v>-9.3788943000000007</v>
+        <v>-15.570838999999999</v>
       </c>
       <c r="F27">
-        <v>-15.357067499999999</v>
+        <v>-4.9544290000000002</v>
       </c>
       <c r="G27">
-        <v>-11.964216800000001</v>
+        <v>-18.15232</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="0"/>
-        <v>-17.023609333333333</v>
+        <v>-15.565160499999999</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>-21.051254400000001</v>
+        <v>-17.024256900000001</v>
       </c>
       <c r="C28">
-        <v>-35.874384800000001</v>
+        <v>-35.764348699999999</v>
       </c>
       <c r="D28">
-        <v>-14.488807400000001</v>
+        <v>-12.6528718</v>
       </c>
       <c r="E28">
-        <v>-15.7279968</v>
+        <v>-9.3788943000000007</v>
       </c>
       <c r="F28">
-        <v>-21.044934699999999</v>
+        <v>-15.357067499999999</v>
       </c>
       <c r="G28">
-        <v>-20.655329399999999</v>
+        <v>-11.964216800000001</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>-21.473784583333337</v>
+        <v>-17.023609333333333</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>-23.006976300000002</v>
+        <v>-21.051254400000001</v>
       </c>
       <c r="C29">
-        <v>-25.191940899999999</v>
+        <v>-35.874384800000001</v>
       </c>
       <c r="D29">
-        <v>-12.8687497</v>
+        <v>-14.488807400000001</v>
       </c>
       <c r="E29">
-        <v>-12.707176199999999</v>
+        <v>-15.7279968</v>
       </c>
       <c r="F29">
-        <v>-16.2397293</v>
+        <v>-21.044934699999999</v>
       </c>
       <c r="G29">
-        <v>-15.251213099999999</v>
+        <v>-20.655329399999999</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="0"/>
-        <v>-17.544297583333332</v>
+        <v>-21.473784583333337</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>-19.459890300000001</v>
+        <v>-23.006976300000002</v>
       </c>
       <c r="C30">
-        <v>-25.9772435</v>
+        <v>-25.191940899999999</v>
       </c>
       <c r="D30">
-        <v>-13.967892600000001</v>
+        <v>-12.8687497</v>
       </c>
       <c r="E30">
-        <v>-16.292657500000001</v>
+        <v>-12.707176199999999</v>
       </c>
       <c r="F30">
-        <v>-8.9381845999999996</v>
+        <v>-16.2397293</v>
       </c>
       <c r="G30">
-        <v>-18.078353199999999</v>
+        <v>-15.251213099999999</v>
       </c>
       <c r="H30" s="3">
         <f t="shared" si="0"/>
-        <v>-17.119036949999998</v>
+        <v>-17.544297583333332</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>-19.459890300000001</v>
+      </c>
+      <c r="C31">
+        <v>-25.9772435</v>
+      </c>
+      <c r="D31">
+        <v>-13.967892600000001</v>
+      </c>
+      <c r="E31">
+        <v>-16.292657500000001</v>
+      </c>
+      <c r="F31">
+        <v>-8.9381845999999996</v>
+      </c>
+      <c r="G31">
+        <v>-18.078353199999999</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="0"/>
+        <v>-17.119036949999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>-24.278553299999999</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>-23.9744086</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>-14.940697200000001</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>-19.242381999999999</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>-29.518176700000001</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>-22.701972999999999</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H32" s="4">
         <f t="shared" si="0"/>
         <v>-22.44269846666667</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B31">
+  <conditionalFormatting sqref="B2:B32">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1429,7 +1485,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C31">
+  <conditionalFormatting sqref="C2:C32">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1441,7 +1497,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1453,7 +1509,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1465,7 +1521,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1477,7 +1533,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1489,7 +1545,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
+  <conditionalFormatting sqref="H2">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1501,8 +1557,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="H3:H1048576">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1514,16 +1570,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1537,855 +1593,860 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="29.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>0.64</v>
-      </c>
-      <c r="C2">
-        <v>-3.073</v>
-      </c>
-      <c r="D2">
-        <v>0.48299999999999998</v>
-      </c>
-      <c r="E2">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="F2">
-        <v>-1.766</v>
-      </c>
-      <c r="G2">
-        <v>0.85</v>
-      </c>
-      <c r="H2" s="3">
-        <f>SUM(B2:G2)</f>
-        <v>-2.0189999999999997</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.27600000000000002</v>
+        <v>0.64</v>
       </c>
       <c r="C3">
-        <v>-3.2829999999999999</v>
+        <v>-3.073</v>
       </c>
       <c r="D3">
-        <v>-1392.027</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="E3">
-        <v>-1.044</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="F3">
-        <v>-3.8540000000000001</v>
+        <v>-1.766</v>
       </c>
       <c r="G3">
-        <v>-7.6820000000000004</v>
+        <v>0.85</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H31" si="0">SUM(B3:G3)</f>
-        <v>-1408.1660000000002</v>
+        <f>AVERAGE(B3:G3)</f>
+        <v>-0.33649999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.502</v>
+        <v>-0.27600000000000002</v>
       </c>
       <c r="C4">
-        <v>0.35899999999999999</v>
+        <v>-3.2829999999999999</v>
       </c>
       <c r="D4">
-        <v>0.20599999999999999</v>
+        <v>-1392.027</v>
       </c>
       <c r="E4">
-        <v>0.28000000000000003</v>
+        <v>-1.044</v>
       </c>
       <c r="F4">
-        <v>9.0999999999999998E-2</v>
+        <v>-3.8540000000000001</v>
       </c>
       <c r="G4">
-        <v>0.69299999999999995</v>
+        <v>-7.6820000000000004</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>2.1309999999999998</v>
+        <f t="shared" ref="H4:H32" si="0">AVERAGE(B4:G4)</f>
+        <v>-234.69433333333336</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.34599999999999997</v>
+        <v>0.502</v>
       </c>
       <c r="C5">
-        <v>-5.476</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="D5">
-        <v>-6.9000000000000006E-2</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="E5">
-        <v>-1.0760000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F5">
-        <v>-20.052</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="G5">
-        <v>0.16900000000000001</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>-26.157999999999998</v>
+        <v>0.35516666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>0.158</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C6">
-        <v>-1.5429999999999999</v>
+        <v>-5.476</v>
       </c>
       <c r="D6">
-        <v>-0.218</v>
+        <v>-6.9000000000000006E-2</v>
       </c>
       <c r="E6">
-        <v>-0.187</v>
+        <v>-1.0760000000000001</v>
       </c>
       <c r="F6">
-        <v>-7.1369999999999996</v>
+        <v>-20.052</v>
       </c>
       <c r="G6">
-        <v>-0.27300000000000002</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>-9.1999999999999993</v>
+        <v>-4.3596666666666666</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>0.63400000000000001</v>
+        <v>0.158</v>
       </c>
       <c r="C7">
-        <v>0.14499999999999999</v>
+        <v>-1.5429999999999999</v>
       </c>
       <c r="D7">
-        <v>0.35799999999999998</v>
+        <v>-0.218</v>
       </c>
       <c r="E7">
-        <v>0.73199999999999998</v>
+        <v>-0.187</v>
       </c>
       <c r="F7">
-        <v>-6.5330000000000004</v>
+        <v>-7.1369999999999996</v>
       </c>
       <c r="G7">
-        <v>0.80500000000000005</v>
+        <v>-0.27300000000000002</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>-3.8590000000000004</v>
+        <v>-1.5333333333333332</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.625</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="C8">
-        <v>-1.4890000000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="D8">
-        <v>-0.20399999999999999</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="E8">
-        <v>-0.75700000000000001</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="F8">
-        <v>-0.97699999999999998</v>
+        <v>-6.5330000000000004</v>
       </c>
       <c r="G8">
-        <v>-0.32800000000000001</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
-        <v>-4.3800000000000008</v>
+        <v>-0.64316666666666678</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>0.32</v>
+        <v>-0.625</v>
       </c>
       <c r="C9">
-        <v>-6.8029999999999999</v>
+        <v>-1.4890000000000001</v>
       </c>
       <c r="D9">
-        <v>0.21199999999999999</v>
+        <v>-0.20399999999999999</v>
       </c>
       <c r="E9">
-        <v>0.23200000000000001</v>
+        <v>-0.75700000000000001</v>
       </c>
       <c r="F9">
-        <v>-2.1989999999999998</v>
+        <v>-0.97699999999999998</v>
       </c>
       <c r="G9">
-        <v>0.45500000000000002</v>
+        <v>-0.32800000000000001</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>-7.7829999999999995</v>
+        <v>-0.73000000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>0.15</v>
+        <v>0.32</v>
       </c>
       <c r="C10">
-        <v>-6.9770000000000003</v>
+        <v>-6.8029999999999999</v>
       </c>
       <c r="D10">
-        <v>0.30599999999999999</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="E10">
-        <v>0.372</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="F10">
-        <v>-14.78</v>
+        <v>-2.1989999999999998</v>
       </c>
       <c r="G10">
-        <v>0.625</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>-20.303999999999998</v>
+        <v>-1.2971666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="C11">
-        <v>-37.713999999999999</v>
+        <v>-6.9770000000000003</v>
       </c>
       <c r="D11">
-        <v>0.189</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="E11">
-        <v>0.24099999999999999</v>
+        <v>0.372</v>
       </c>
       <c r="F11">
-        <v>-0.51800000000000002</v>
+        <v>-14.78</v>
       </c>
       <c r="G11">
-        <v>0.44500000000000001</v>
+        <v>0.625</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>-36.856999999999999</v>
+        <v>-3.3839999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>-0.20699999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="C12">
-        <v>-22.071999999999999</v>
+        <v>-37.713999999999999</v>
       </c>
       <c r="D12">
-        <v>0.16</v>
+        <v>0.189</v>
       </c>
       <c r="E12">
-        <v>-0.47399999999999998</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="F12">
-        <v>-4.8259999999999996</v>
+        <v>-0.51800000000000002</v>
       </c>
       <c r="G12">
-        <v>0.23200000000000001</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="0"/>
-        <v>-27.187000000000001</v>
+        <v>-6.1428333333333329</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>0.71</v>
+        <v>-0.20699999999999999</v>
       </c>
       <c r="C13">
-        <v>-3.0840000000000001</v>
+        <v>-22.071999999999999</v>
       </c>
       <c r="D13">
-        <v>0.32200000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="E13">
-        <v>0.115</v>
+        <v>-0.47399999999999998</v>
       </c>
       <c r="F13">
-        <v>-3.9550000000000001</v>
+        <v>-4.8259999999999996</v>
       </c>
       <c r="G13">
-        <v>0.23400000000000001</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="0"/>
-        <v>-5.6580000000000004</v>
+        <v>-4.5311666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>0.755</v>
+        <v>0.71</v>
       </c>
       <c r="C14">
-        <v>-35.832999999999998</v>
+        <v>-3.0840000000000001</v>
       </c>
       <c r="D14">
-        <v>0.315</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="E14">
-        <v>0.27400000000000002</v>
+        <v>0.115</v>
       </c>
       <c r="F14">
-        <v>-15.532</v>
+        <v>-3.9550000000000001</v>
       </c>
       <c r="G14">
-        <v>0.48199999999999998</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="0"/>
-        <v>-49.539000000000001</v>
+        <v>-0.94300000000000006</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>0.48899999999999999</v>
+        <v>0.755</v>
       </c>
       <c r="C15">
-        <v>-59.792999999999999</v>
+        <v>-35.832999999999998</v>
       </c>
       <c r="D15">
-        <v>0.309</v>
+        <v>0.315</v>
       </c>
       <c r="E15">
-        <v>0.76</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="F15">
-        <v>-15.16</v>
+        <v>-15.532</v>
       </c>
       <c r="G15">
-        <v>0.76300000000000001</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="0"/>
-        <v>-72.632000000000005</v>
+        <v>-8.2565000000000008</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>0.59599999999999997</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="C16">
-        <v>-10.510999999999999</v>
+        <v>-59.792999999999999</v>
       </c>
       <c r="D16">
-        <v>0.34399999999999997</v>
+        <v>0.309</v>
       </c>
       <c r="E16">
-        <v>0.435</v>
+        <v>0.76</v>
       </c>
       <c r="F16">
-        <v>-0.248</v>
+        <v>-15.16</v>
       </c>
       <c r="G16">
-        <v>0.58199999999999996</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="0"/>
-        <v>-8.8019999999999978</v>
+        <v>-12.105333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>0.52300000000000002</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="C17">
-        <v>-1.123</v>
+        <v>-10.510999999999999</v>
       </c>
       <c r="D17">
-        <v>0.13700000000000001</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="E17">
-        <v>-1.909</v>
+        <v>0.435</v>
       </c>
       <c r="F17">
-        <v>-14.901</v>
+        <v>-0.248</v>
       </c>
       <c r="G17">
-        <v>0.46500000000000002</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="0"/>
-        <v>-16.808</v>
+        <v>-1.4669999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>0.43099999999999999</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="C18">
-        <v>-1.569</v>
+        <v>-1.123</v>
       </c>
       <c r="D18">
-        <v>3.7999999999999999E-2</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E18">
-        <v>-0.58799999999999997</v>
+        <v>-1.909</v>
       </c>
       <c r="F18">
-        <v>-14.455</v>
+        <v>-14.901</v>
       </c>
       <c r="G18">
-        <v>0.28599999999999998</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="H18" s="3">
         <f t="shared" si="0"/>
-        <v>-15.857000000000001</v>
+        <v>-2.8013333333333335</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>0.68700000000000006</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="C19">
-        <v>-123.502</v>
+        <v>-1.569</v>
       </c>
       <c r="D19">
-        <v>0.29399999999999998</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E19">
-        <v>-0.95699999999999996</v>
+        <v>-0.58799999999999997</v>
       </c>
       <c r="F19">
-        <v>-34.518999999999998</v>
+        <v>-14.455</v>
       </c>
       <c r="G19">
-        <v>0.65700000000000003</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="0"/>
-        <v>-157.33999999999997</v>
+        <v>-2.6428333333333334</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>0.64100000000000001</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="C20">
-        <v>0.40899999999999997</v>
+        <v>-123.502</v>
       </c>
       <c r="D20">
-        <v>0.39100000000000001</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="E20">
-        <v>0.124</v>
+        <v>-0.95699999999999996</v>
       </c>
       <c r="F20">
-        <v>-1.091</v>
+        <v>-34.518999999999998</v>
       </c>
       <c r="G20">
-        <v>0.71899999999999997</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="0"/>
-        <v>1.1930000000000001</v>
+        <v>-26.223333333333329</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>0.115</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="C21">
-        <v>-6.8540000000000001</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="D21">
-        <v>0.21</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="E21">
-        <v>2.7E-2</v>
+        <v>0.124</v>
       </c>
       <c r="F21">
-        <v>-12.29</v>
+        <v>-1.091</v>
       </c>
       <c r="G21">
-        <v>7.4999999999999997E-2</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="0"/>
-        <v>-18.716999999999999</v>
+        <v>0.19883333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>0.82599999999999996</v>
+        <v>0.115</v>
       </c>
       <c r="C22">
-        <v>-48.878</v>
+        <v>-6.8540000000000001</v>
       </c>
       <c r="D22">
-        <v>0.51900000000000002</v>
+        <v>0.21</v>
       </c>
       <c r="E22">
-        <v>0.85699999999999998</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F22">
-        <v>-16.427</v>
+        <v>-12.29</v>
       </c>
       <c r="G22">
-        <v>0.89600000000000002</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="0"/>
-        <v>-62.207000000000001</v>
+        <v>-3.1194999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>0.59199999999999997</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="C23">
-        <v>-0.60499999999999998</v>
+        <v>-48.878</v>
       </c>
       <c r="D23">
-        <v>0.153</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="E23">
-        <v>-0.24399999999999999</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="F23">
-        <v>-0.42699999999999999</v>
+        <v>-16.427</v>
       </c>
       <c r="G23">
-        <v>0.65900000000000003</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" si="0"/>
-        <v>0.128</v>
+        <v>-10.367833333333333</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>0.55200000000000005</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="C24">
-        <v>-36.090000000000003</v>
+        <v>-0.60499999999999998</v>
       </c>
       <c r="D24">
-        <v>0.39500000000000002</v>
+        <v>0.153</v>
       </c>
       <c r="E24">
-        <v>0.76500000000000001</v>
+        <v>-0.24399999999999999</v>
       </c>
       <c r="F24">
-        <v>-28.056000000000001</v>
+        <v>-0.42699999999999999</v>
       </c>
       <c r="G24">
-        <v>0.4</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="0"/>
-        <v>-62.033999999999999</v>
+        <v>2.1333333333333333E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>0.58699999999999997</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="C25">
-        <v>-56.161999999999999</v>
+        <v>-36.090000000000003</v>
       </c>
       <c r="D25">
-        <v>0.41199999999999998</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="E25">
-        <v>0.17399999999999999</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="F25">
-        <v>0.32700000000000001</v>
+        <v>-28.056000000000001</v>
       </c>
       <c r="G25">
-        <v>0.56399999999999995</v>
+        <v>0.4</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="0"/>
-        <v>-54.097999999999999</v>
+        <v>-10.339</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>0.70399999999999996</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="C26">
-        <v>-131.82499999999999</v>
+        <v>-56.161999999999999</v>
       </c>
       <c r="D26">
-        <v>0.16400000000000001</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="E26">
-        <v>0.45200000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F26">
-        <v>-83.959000000000003</v>
+        <v>0.32700000000000001</v>
       </c>
       <c r="G26">
-        <v>0.61</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="0"/>
-        <v>-213.85399999999998</v>
+        <v>-9.0163333333333338</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>0.105</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="C27">
-        <v>-2.2679999999999998</v>
+        <v>-131.82499999999999</v>
       </c>
       <c r="D27">
-        <v>5.0999999999999997E-2</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="E27">
-        <v>-1.2809999999999999</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="F27">
-        <v>-6.7439999999999998</v>
+        <v>-83.959000000000003</v>
       </c>
       <c r="G27">
-        <v>-0.623</v>
+        <v>0.61</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="0"/>
-        <v>-10.76</v>
+        <v>-35.642333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
-        <v>0.64600000000000002</v>
+        <v>0.105</v>
       </c>
       <c r="C28">
-        <v>-2.1859999999999999</v>
+        <v>-2.2679999999999998</v>
       </c>
       <c r="D28">
-        <v>0.378</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E28">
-        <v>0.47099999999999997</v>
+        <v>-1.2809999999999999</v>
       </c>
       <c r="F28">
-        <v>-1.0900000000000001</v>
+        <v>-6.7439999999999998</v>
       </c>
       <c r="G28">
-        <v>0.78100000000000003</v>
+        <v>-0.623</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-1.7933333333333332</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29">
-        <v>0.77400000000000002</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="C29">
-        <v>-36.286999999999999</v>
+        <v>-2.1859999999999999</v>
       </c>
       <c r="D29">
-        <v>9.7000000000000003E-2</v>
+        <v>0.378</v>
       </c>
       <c r="E29">
-        <v>-0.06</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="F29">
-        <v>-5.319</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="G29">
-        <v>0.23799999999999999</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="0"/>
-        <v>-40.557000000000002</v>
+        <v>-0.16666666666666666</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>0.48899999999999999</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="C30">
-        <v>-30.119</v>
+        <v>-36.286999999999999</v>
       </c>
       <c r="D30">
-        <v>0.29899999999999999</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="E30">
-        <v>0.53600000000000003</v>
+        <v>-0.06</v>
       </c>
       <c r="F30">
-        <v>-32.948999999999998</v>
+        <v>-5.319</v>
       </c>
       <c r="G30">
-        <v>0.60299999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="H30" s="3">
         <f t="shared" si="0"/>
-        <v>-61.140999999999998</v>
+        <v>-6.7595000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C31">
+        <v>-30.119</v>
+      </c>
+      <c r="D31">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E31">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F31">
+        <v>-32.948999999999998</v>
+      </c>
+      <c r="G31">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="0"/>
+        <v>-10.190166666666666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>0.83199999999999996</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>-48.353000000000002</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>0.44</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>0.76500000000000001</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>0.70299999999999996</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>0.86299999999999999</v>
       </c>
-      <c r="H31" s="4">
-        <f t="shared" si="0"/>
-        <v>-44.75</v>
+      <c r="H32" s="3">
+        <f t="shared" si="0"/>
+        <v>-7.458333333333333</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B31">
+  <conditionalFormatting sqref="B3:B32">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="40">
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2395,38 +2456,58 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C31">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="C3:C32">
     <cfRule type="colorScale" priority="10">
       <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="30"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="20"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
@@ -2435,37 +2516,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="D3:D32">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2475,37 +2556,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E31">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="E3:E32">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2515,37 +2596,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F31">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="F3:F32">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2555,37 +2636,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="G3:G32">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2595,37 +2676,37 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$2:$B$31-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="H3:H32">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
         <cfvo type="percentile" val="50"/>
@@ -2635,22 +2716,94 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$2:$B$31))"/>
-        <cfvo type="formula" val="MAX(ABS($B$2:$B$31))"/>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Almost all Autoformer rsults uploaded. Metrics Permittiviti fixed
</commit_message>
<xml_diff>
--- a/TFG_Results/Transformer_results/Transformer_metrics.xlsx
+++ b/TFG_Results/Transformer_results/Transformer_metrics.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\OneDrive\Escritorio\TFG_TST\TFG_Results\Transformer_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4D7186-193A-4206-B350-A01F348A924C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01002F6-07AE-43C1-8DEB-E469E8F0C376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2610" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSE" sheetId="1" r:id="rId1"/>
     <sheet name="R_squared" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MSE!$K$2:$S$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">R_squared!$K$2:$S$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="43">
   <si>
     <t>Folder</t>
   </si>
@@ -46,6 +50,9 @@
   </si>
   <si>
     <t>Light</t>
+  </si>
+  <si>
+    <t>Permittivity</t>
   </si>
   <si>
     <t>Relative_humidity</t>
@@ -158,9 +165,8 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <vertAlign val="superscript"/>
-        <sz val="20"/>
+        <sz val="22"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -169,12 +175,18 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>Sorted by model</t>
+  </si>
+  <si>
+    <t>Sorted by Diameter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,33 +201,15 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <vertAlign val="superscript"/>
-      <sz val="20"/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -230,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -284,9 +278,31 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -294,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -303,13 +319,19 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,29 +635,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,16 +708,46 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>-21.032771</v>
@@ -675,22 +759,53 @@
         <v>-15.533721699999999</v>
       </c>
       <c r="E3">
+        <v>-27.477354900000002</v>
+      </c>
+      <c r="F3">
         <v>-20.932425800000001</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>-20.5435844</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-22.3636421</v>
       </c>
-      <c r="H3" s="3">
-        <f>AVERAGE(B3:G3)</f>
-        <v>-22.736206233333334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="3">
+        <f>AVERAGE(B3:H3)</f>
+        <v>-23.413513185714287</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>-24.278553299999999</v>
+      </c>
+      <c r="M3">
+        <v>-23.9744086</v>
+      </c>
+      <c r="N3">
+        <v>-14.940697200000001</v>
+      </c>
+      <c r="O3">
+        <v>-17.899998</v>
+      </c>
+      <c r="P3">
+        <v>-19.242381999999999</v>
+      </c>
+      <c r="Q3">
+        <v>-29.518176700000001</v>
+      </c>
+      <c r="R3">
+        <v>-22.701972999999999</v>
+      </c>
+      <c r="S3" s="3">
+        <f>AVERAGE(L3:R3)</f>
+        <v>-21.793741257142859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>-20.406924400000001</v>
@@ -702,22 +817,53 @@
         <v>-24.157681199999999</v>
       </c>
       <c r="E4">
+        <v>-30.0255689</v>
+      </c>
+      <c r="F4">
         <v>-19.944791500000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>-19.389690699999999</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-18.658907200000002</v>
       </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H32" si="0">AVERAGE(B4:G4)</f>
-        <v>-23.934649816666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="3">
+        <f>AVERAGE(B4:H4)</f>
+        <v>-24.804781114285714</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>-24.135540899999999</v>
+      </c>
+      <c r="M4">
+        <v>-23.9283909</v>
+      </c>
+      <c r="N4">
+        <v>-15.604567299999999</v>
+      </c>
+      <c r="O4">
+        <v>-21.132429200000001</v>
+      </c>
+      <c r="P4">
+        <v>-21.3973215</v>
+      </c>
+      <c r="Q4">
+        <v>-11.8342948</v>
+      </c>
+      <c r="R4">
+        <v>-23.898673800000001</v>
+      </c>
+      <c r="S4" s="3">
+        <f>AVERAGE(L4:R4)</f>
+        <v>-20.275888342857144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>-19.570627399999999</v>
@@ -729,22 +875,53 @@
         <v>-13.427972199999999</v>
       </c>
       <c r="E5">
+        <v>-22.449071199999999</v>
+      </c>
+      <c r="F5">
         <v>-14.385999</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>-24.658665500000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>-19.191879</v>
       </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>-22.346108049999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="3">
+        <f>AVERAGE(B5:H5)</f>
+        <v>-22.360817071428574</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>-23.006976300000002</v>
+      </c>
+      <c r="M5">
+        <v>-25.191940899999999</v>
+      </c>
+      <c r="N5">
+        <v>-12.8687497</v>
+      </c>
+      <c r="O5">
+        <v>-25.025856900000001</v>
+      </c>
+      <c r="P5">
+        <v>-12.707176199999999</v>
+      </c>
+      <c r="Q5">
+        <v>-16.2397293</v>
+      </c>
+      <c r="R5">
+        <v>-15.251213099999999</v>
+      </c>
+      <c r="S5" s="3">
+        <f>AVERAGE(L5:R5)</f>
+        <v>-18.613091771428572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>-17.294701199999999</v>
@@ -756,22 +933,53 @@
         <v>-12.6093098</v>
       </c>
       <c r="E6">
+        <v>-23.0112609</v>
+      </c>
+      <c r="F6">
         <v>-9.8376903999999996</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>-10.601813699999999</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>-14.606989</v>
       </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>-15.90702508333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="3">
+        <f>AVERAGE(B6:H6)</f>
+        <v>-16.921915914285712</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>-22.651688400000001</v>
+      </c>
+      <c r="M6">
+        <v>-25.245136800000001</v>
+      </c>
+      <c r="N6">
+        <v>-14.0649937</v>
+      </c>
+      <c r="O6">
+        <v>-21.347769100000001</v>
+      </c>
+      <c r="P6">
+        <v>-14.3514952</v>
+      </c>
+      <c r="Q6">
+        <v>-12.0631833</v>
+      </c>
+      <c r="R6">
+        <v>-16.922112500000001</v>
+      </c>
+      <c r="S6" s="3">
+        <f>AVERAGE(L6:R6)</f>
+        <v>-18.092339857142857</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>-17.2872588</v>
@@ -783,22 +991,53 @@
         <v>-11.5675398</v>
       </c>
       <c r="E7">
+        <v>-24.689225</v>
+      </c>
+      <c r="F7">
         <v>-12.2167098</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>-15.1419671</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-13.018887899999999</v>
       </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.681163300000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="3">
+        <f>AVERAGE(B7:H7)</f>
+        <v>-18.682314971428575</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7">
+        <v>-21.9155008</v>
+      </c>
+      <c r="M7">
+        <v>-34.797186600000003</v>
+      </c>
+      <c r="N7">
+        <v>-14.1095326</v>
+      </c>
+      <c r="O7">
+        <v>-27.610312499999999</v>
+      </c>
+      <c r="P7">
+        <v>-13.4932493</v>
+      </c>
+      <c r="Q7">
+        <v>-17.295736099999999</v>
+      </c>
+      <c r="R7">
+        <v>-15.225873399999999</v>
+      </c>
+      <c r="S7" s="3">
+        <f>AVERAGE(L7:R7)</f>
+        <v>-20.635341614285718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>-20.911200900000001</v>
@@ -810,22 +1049,53 @@
         <v>-14.3505067</v>
       </c>
       <c r="E8">
+        <v>-30.261843899999999</v>
+      </c>
+      <c r="F8">
         <v>-18.6842568</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>-15.477086999999999</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>-21.170314000000001</v>
       </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>-22.030242183333332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="3">
+        <f>AVERAGE(B8:H8)</f>
+        <v>-23.206185285714287</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>-21.835591999999998</v>
+      </c>
+      <c r="M8">
+        <v>-19.674721999999999</v>
+      </c>
+      <c r="N8">
+        <v>-13.203061</v>
+      </c>
+      <c r="O8">
+        <v>-9.5199739999999995</v>
+      </c>
+      <c r="P8">
+        <v>-15.570838999999999</v>
+      </c>
+      <c r="Q8">
+        <v>-4.9544290000000002</v>
+      </c>
+      <c r="R8">
+        <v>-18.15232</v>
+      </c>
+      <c r="S8" s="3">
+        <f>AVERAGE(L8:R8)</f>
+        <v>-14.701562428571426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>-14.4346215</v>
@@ -837,22 +1107,53 @@
         <v>-11.6185954</v>
       </c>
       <c r="E9">
+        <v>-26.387392500000001</v>
+      </c>
+      <c r="F9">
         <v>-10.512088500000001</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>-21.2859129</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>-12.835842599999999</v>
       </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.938974866666669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="3">
+        <f>AVERAGE(B9:H9)</f>
+        <v>-19.145891671428576</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>-21.5816029</v>
+      </c>
+      <c r="M9">
+        <v>-19.955765599999999</v>
+      </c>
+      <c r="N9">
+        <v>-13.933817700000001</v>
+      </c>
+      <c r="O9">
+        <v>-9.3935507000000005</v>
+      </c>
+      <c r="P9">
+        <v>-10.044253100000001</v>
+      </c>
+      <c r="Q9">
+        <v>-8.7419446999999995</v>
+      </c>
+      <c r="R9">
+        <v>-18.710442499999999</v>
+      </c>
+      <c r="S9" s="3">
+        <f>AVERAGE(L9:R9)</f>
+        <v>-14.623053885714286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>-18.2175999</v>
@@ -864,22 +1165,53 @@
         <v>-13.4595447</v>
       </c>
       <c r="E10">
+        <v>-30.2985352</v>
+      </c>
+      <c r="F10">
         <v>-14.109465500000001</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-19.196473399999999</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-16.701698100000002</v>
       </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>-18.94491446666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="3">
+        <f>AVERAGE(B10:H10)</f>
+        <v>-20.566860285714288</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10">
+        <v>-21.051254400000001</v>
+      </c>
+      <c r="M10">
+        <v>-35.874384800000001</v>
+      </c>
+      <c r="N10">
+        <v>-14.488807400000001</v>
+      </c>
+      <c r="O10">
+        <v>-25.819765799999999</v>
+      </c>
+      <c r="P10">
+        <v>-15.7279968</v>
+      </c>
+      <c r="Q10">
+        <v>-21.044934699999999</v>
+      </c>
+      <c r="R10">
+        <v>-20.655329399999999</v>
+      </c>
+      <c r="S10" s="3">
+        <f>AVERAGE(L10:R10)</f>
+        <v>-22.094639042857146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>-17.250018699999998</v>
@@ -891,22 +1223,53 @@
         <v>-14.0132931</v>
       </c>
       <c r="E11">
+        <v>-17.640318300000001</v>
+      </c>
+      <c r="F11">
         <v>-14.982514200000001</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>-12.2655283</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>-18.328409300000001</v>
       </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>-18.121454566666667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="3">
+        <f>AVERAGE(B11:H11)</f>
+        <v>-18.052720814285713</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>-21.032771</v>
+      </c>
+      <c r="M11">
+        <v>-36.011092400000003</v>
+      </c>
+      <c r="N11">
+        <v>-15.533721699999999</v>
+      </c>
+      <c r="O11">
+        <v>-27.477354900000002</v>
+      </c>
+      <c r="P11">
+        <v>-20.932425800000001</v>
+      </c>
+      <c r="Q11">
+        <v>-20.5435844</v>
+      </c>
+      <c r="R11">
+        <v>-22.3636421</v>
+      </c>
+      <c r="S11" s="3">
+        <f>AVERAGE(L11:R11)</f>
+        <v>-23.413513185714287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>-19.5548067</v>
@@ -918,22 +1281,53 @@
         <v>-13.334423900000001</v>
       </c>
       <c r="E12">
+        <v>-31.577105599999999</v>
+      </c>
+      <c r="F12">
         <v>-14.161092699999999</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-22.432455399999998</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>-16.625015600000001</v>
       </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>-18.52278085</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="3">
+        <f>AVERAGE(B12:H12)</f>
+        <v>-20.387684385714287</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12">
+        <v>-20.989706399999999</v>
+      </c>
+      <c r="M12">
+        <v>-43.193805500000003</v>
+      </c>
+      <c r="N12">
+        <v>-14.5751621</v>
+      </c>
+      <c r="O12">
+        <v>-23.413073600000001</v>
+      </c>
+      <c r="P12">
+        <v>-13.536150599999999</v>
+      </c>
+      <c r="Q12">
+        <v>-21.043924100000002</v>
+      </c>
+      <c r="R12">
+        <v>-19.5807295</v>
+      </c>
+      <c r="S12" s="3">
+        <f>AVERAGE(L12:R12)</f>
+        <v>-22.333221685714285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>-15.7261474</v>
@@ -945,22 +1339,53 @@
         <v>-13.1792315</v>
       </c>
       <c r="E13">
+        <v>-24.939641999999999</v>
+      </c>
+      <c r="F13">
         <v>-11.275166199999999</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>-16.593104499999999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>-15.2160967</v>
       </c>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>-16.544416083333331</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="3">
+        <f>AVERAGE(B13:H13)</f>
+        <v>-17.74373407142857</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>-20.911200900000001</v>
+      </c>
+      <c r="M13">
+        <v>-41.588087700000003</v>
+      </c>
+      <c r="N13">
+        <v>-14.3505067</v>
+      </c>
+      <c r="O13">
+        <v>-30.261843899999999</v>
+      </c>
+      <c r="P13">
+        <v>-18.6842568</v>
+      </c>
+      <c r="Q13">
+        <v>-15.477086999999999</v>
+      </c>
+      <c r="R13">
+        <v>-21.170314000000001</v>
+      </c>
+      <c r="S13" s="3">
+        <f>AVERAGE(L13:R13)</f>
+        <v>-23.206185285714287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>-21.9155008</v>
@@ -972,22 +1397,53 @@
         <v>-14.1095326</v>
       </c>
       <c r="E14">
+        <v>-27.610312499999999</v>
+      </c>
+      <c r="F14">
         <v>-13.4932493</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-17.295736099999999</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>-15.225873399999999</v>
       </c>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>-19.472846466666667</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="3">
+        <f>AVERAGE(B14:H14)</f>
+        <v>-20.635341614285718</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14">
+        <v>-20.476213999999999</v>
+      </c>
+      <c r="M14">
+        <v>-30.296253199999999</v>
+      </c>
+      <c r="N14">
+        <v>-14.2529889</v>
+      </c>
+      <c r="O14">
+        <v>-34.5703502</v>
+      </c>
+      <c r="P14">
+        <v>-15.438332000000001</v>
+      </c>
+      <c r="Q14">
+        <v>-23.2839563</v>
+      </c>
+      <c r="R14">
+        <v>-17.853883700000001</v>
+      </c>
+      <c r="S14" s="3">
+        <f>AVERAGE(L14:R14)</f>
+        <v>-22.310282614285715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>-22.651688400000001</v>
@@ -999,22 +1455,53 @@
         <v>-14.0649937</v>
       </c>
       <c r="E15">
+        <v>-21.347769100000001</v>
+      </c>
+      <c r="F15">
         <v>-14.3514952</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-12.0631833</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>-16.922112500000001</v>
       </c>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.549768316666668</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="3">
+        <f>AVERAGE(B15:H15)</f>
+        <v>-18.092339857142857</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15">
+        <v>-20.433776999999999</v>
+      </c>
+      <c r="M15">
+        <v>-38.852964299999996</v>
+      </c>
+      <c r="N15">
+        <v>-13.1445095</v>
+      </c>
+      <c r="O15">
+        <v>-29.004337899999999</v>
+      </c>
+      <c r="P15">
+        <v>-12.014249299999999</v>
+      </c>
+      <c r="Q15">
+        <v>-22.7017396</v>
+      </c>
+      <c r="R15">
+        <v>-18.745516299999998</v>
+      </c>
+      <c r="S15" s="3">
+        <f>AVERAGE(L15:R15)</f>
+        <v>-22.128156271428569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>-19.461395199999998</v>
@@ -1026,22 +1513,53 @@
         <v>-14.026277800000001</v>
       </c>
       <c r="E16">
+        <v>-5.4594525000000003</v>
+      </c>
+      <c r="F16">
         <v>-19.150310300000001</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>-12.1621197</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>-20.3138197</v>
       </c>
-      <c r="H16" s="3">
-        <f t="shared" si="0"/>
-        <v>-18.030488033333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="3">
+        <f>AVERAGE(B16:H16)</f>
+        <v>-16.234625814285714</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16">
+        <v>-20.406924400000001</v>
+      </c>
+      <c r="M16">
+        <v>-41.049903899999997</v>
+      </c>
+      <c r="N16">
+        <v>-24.157681199999999</v>
+      </c>
+      <c r="O16">
+        <v>-30.0255689</v>
+      </c>
+      <c r="P16">
+        <v>-19.944791500000001</v>
+      </c>
+      <c r="Q16">
+        <v>-19.389690699999999</v>
+      </c>
+      <c r="R16">
+        <v>-18.658907200000002</v>
+      </c>
+      <c r="S16" s="3">
+        <f>AVERAGE(L16:R16)</f>
+        <v>-24.804781114285714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>-20.476213999999999</v>
@@ -1053,22 +1571,53 @@
         <v>-14.2529889</v>
       </c>
       <c r="E17">
+        <v>-34.5703502</v>
+      </c>
+      <c r="F17">
         <v>-15.438332000000001</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>-23.2839563</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>-17.853883700000001</v>
       </c>
-      <c r="H17" s="3">
-        <f t="shared" si="0"/>
-        <v>-20.266938016666668</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="3">
+        <f>AVERAGE(B17:H17)</f>
+        <v>-22.310282614285715</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <v>-20.381800500000001</v>
+      </c>
+      <c r="M17">
+        <v>-23.336405299999999</v>
+      </c>
+      <c r="N17">
+        <v>-14.7327732</v>
+      </c>
+      <c r="O17">
+        <v>-14.506357700000001</v>
+      </c>
+      <c r="P17">
+        <v>-13.7929718</v>
+      </c>
+      <c r="Q17">
+        <v>-25.966559100000001</v>
+      </c>
+      <c r="R17">
+        <v>-17.677706400000002</v>
+      </c>
+      <c r="S17" s="3">
+        <f>AVERAGE(L17:R17)</f>
+        <v>-18.627796285714286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>-19.754861399999999</v>
@@ -1080,22 +1629,53 @@
         <v>-13.064559300000001</v>
       </c>
       <c r="E18">
+        <v>-24.5383557</v>
+      </c>
+      <c r="F18">
         <v>-8.3234320999999998</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>-12.232351700000001</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>-16.7883104</v>
       </c>
-      <c r="H18" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.966898400000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="3">
+        <f>AVERAGE(B18:H18)</f>
+        <v>-18.905678014285716</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18">
+        <v>-20.025093699999999</v>
+      </c>
+      <c r="M18">
+        <v>-25.214934</v>
+      </c>
+      <c r="N18">
+        <v>-14.6063376</v>
+      </c>
+      <c r="O18">
+        <v>-12.9488445</v>
+      </c>
+      <c r="P18">
+        <v>-19.2521974</v>
+      </c>
+      <c r="Q18">
+        <v>-9.6140931999999992</v>
+      </c>
+      <c r="R18">
+        <v>-16.289753099999999</v>
+      </c>
+      <c r="S18" s="3">
+        <f>AVERAGE(L18:R18)</f>
+        <v>-16.850179071428574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>-18.992035900000001</v>
@@ -1107,22 +1687,53 @@
         <v>-12.5907407</v>
       </c>
       <c r="E19">
+        <v>-27.6245911</v>
+      </c>
+      <c r="F19">
         <v>-10.951613699999999</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>-12.355860099999999</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>-15.5308291</v>
       </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.871703333333333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="3">
+        <f>AVERAGE(B19:H19)</f>
+        <v>-19.264973014285715</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19">
+        <v>-19.754861399999999</v>
+      </c>
+      <c r="M19">
+        <v>-37.6378755</v>
+      </c>
+      <c r="N19">
+        <v>-13.064559300000001</v>
+      </c>
+      <c r="O19">
+        <v>-24.5383557</v>
+      </c>
+      <c r="P19">
+        <v>-8.3234320999999998</v>
+      </c>
+      <c r="Q19">
+        <v>-12.232351700000001</v>
+      </c>
+      <c r="R19">
+        <v>-16.7883104</v>
+      </c>
+      <c r="S19" s="3">
+        <f>AVERAGE(L19:R19)</f>
+        <v>-18.905678014285716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>-21.5816029</v>
@@ -1134,23 +1745,53 @@
         <v>-13.933817700000001</v>
       </c>
       <c r="E20">
+        <v>-9.3935507000000005</v>
+      </c>
+      <c r="F20">
         <v>-10.044253100000001</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>-8.7419446999999995</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>-18.710442499999999</v>
       </c>
-      <c r="H20" s="3">
-        <f t="shared" si="0"/>
-        <v>-15.494637750000001</v>
-      </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="3">
+        <f>AVERAGE(B20:H20)</f>
+        <v>-14.623053885714286</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>-19.570627399999999</v>
+      </c>
+      <c r="M20">
+        <v>-42.8415052</v>
+      </c>
+      <c r="N20">
+        <v>-13.427972199999999</v>
+      </c>
+      <c r="O20">
+        <v>-22.449071199999999</v>
+      </c>
+      <c r="P20">
+        <v>-14.385999</v>
+      </c>
+      <c r="Q20">
+        <v>-24.658665500000001</v>
+      </c>
+      <c r="R20">
+        <v>-19.191879</v>
+      </c>
+      <c r="S20" s="3">
+        <f>AVERAGE(L20:R20)</f>
+        <v>-22.360817071428574</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>-20.989706399999999</v>
@@ -1162,22 +1803,53 @@
         <v>-14.5751621</v>
       </c>
       <c r="E21">
+        <v>-23.413073600000001</v>
+      </c>
+      <c r="F21">
         <v>-13.536150599999999</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>-21.043924100000002</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>-19.5807295</v>
       </c>
-      <c r="H21" s="3">
-        <f t="shared" si="0"/>
-        <v>-22.153246366666664</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="3">
+        <f>AVERAGE(B21:H21)</f>
+        <v>-22.333221685714285</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21">
+        <v>-19.5548067</v>
+      </c>
+      <c r="M21">
+        <v>-25.028890799999999</v>
+      </c>
+      <c r="N21">
+        <v>-13.334423900000001</v>
+      </c>
+      <c r="O21">
+        <v>-31.577105599999999</v>
+      </c>
+      <c r="P21">
+        <v>-14.161092699999999</v>
+      </c>
+      <c r="Q21">
+        <v>-22.432455399999998</v>
+      </c>
+      <c r="R21">
+        <v>-16.625015600000001</v>
+      </c>
+      <c r="S21" s="3">
+        <f>AVERAGE(L21:R21)</f>
+        <v>-20.387684385714287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>-17.071313199999999</v>
@@ -1189,22 +1861,53 @@
         <v>-13.4470721</v>
       </c>
       <c r="E22">
+        <v>-18.5957328</v>
+      </c>
+      <c r="F22">
         <v>-13.079902499999999</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>-13.011406300000001</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>-14.4059046</v>
       </c>
-      <c r="H22" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.162026833333332</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="3">
+        <f>AVERAGE(B22:H22)</f>
+        <v>-17.366841971428574</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22">
+        <v>-19.461395199999998</v>
+      </c>
+      <c r="M22">
+        <v>-23.069005499999999</v>
+      </c>
+      <c r="N22">
+        <v>-14.026277800000001</v>
+      </c>
+      <c r="O22">
+        <v>-5.4594525000000003</v>
+      </c>
+      <c r="P22">
+        <v>-19.150310300000001</v>
+      </c>
+      <c r="Q22">
+        <v>-12.1621197</v>
+      </c>
+      <c r="R22">
+        <v>-20.3138197</v>
+      </c>
+      <c r="S22" s="3">
+        <f>AVERAGE(L22:R22)</f>
+        <v>-16.234625814285714</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>-24.135540899999999</v>
@@ -1216,22 +1919,53 @@
         <v>-15.604567299999999</v>
       </c>
       <c r="E23">
+        <v>-21.132429200000001</v>
+      </c>
+      <c r="F23">
         <v>-21.3973215</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>-11.8342948</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>-23.898673800000001</v>
       </c>
-      <c r="H23" s="3">
-        <f t="shared" si="0"/>
-        <v>-20.13313153333333</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="3">
+        <f>AVERAGE(B23:H23)</f>
+        <v>-20.275888342857144</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23">
+        <v>-19.459890300000001</v>
+      </c>
+      <c r="M23">
+        <v>-25.9772435</v>
+      </c>
+      <c r="N23">
+        <v>-13.967892600000001</v>
+      </c>
+      <c r="O23">
+        <v>-12.4247824</v>
+      </c>
+      <c r="P23">
+        <v>-16.292657500000001</v>
+      </c>
+      <c r="Q23">
+        <v>-8.9381845999999996</v>
+      </c>
+      <c r="R23">
+        <v>-18.078353199999999</v>
+      </c>
+      <c r="S23" s="3">
+        <f>AVERAGE(L23:R23)</f>
+        <v>-16.448429157142858</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>-20.433776999999999</v>
@@ -1243,22 +1977,53 @@
         <v>-13.1445095</v>
       </c>
       <c r="E24">
+        <v>-29.004337899999999</v>
+      </c>
+      <c r="F24">
         <v>-12.014249299999999</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>-22.7017396</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>-18.745516299999998</v>
       </c>
-      <c r="H24" s="3">
-        <f t="shared" si="0"/>
-        <v>-20.982125999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="3">
+        <f>AVERAGE(B24:H24)</f>
+        <v>-22.128156271428569</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24">
+        <v>-18.992035900000001</v>
+      </c>
+      <c r="M24">
+        <v>-36.809140499999998</v>
+      </c>
+      <c r="N24">
+        <v>-12.5907407</v>
+      </c>
+      <c r="O24">
+        <v>-27.6245911</v>
+      </c>
+      <c r="P24">
+        <v>-10.951613699999999</v>
+      </c>
+      <c r="Q24">
+        <v>-12.355860099999999</v>
+      </c>
+      <c r="R24">
+        <v>-15.5308291</v>
+      </c>
+      <c r="S24" s="3">
+        <f>AVERAGE(L24:R24)</f>
+        <v>-19.264973014285715</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>-20.025093699999999</v>
@@ -1270,22 +2035,53 @@
         <v>-14.6063376</v>
       </c>
       <c r="E25">
+        <v>-12.9488445</v>
+      </c>
+      <c r="F25">
         <v>-19.2521974</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>-9.6140931999999992</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>-16.289753099999999</v>
       </c>
-      <c r="H25" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.500401499999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="3">
+        <f>AVERAGE(B25:H25)</f>
+        <v>-16.850179071428574</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25">
+        <v>-18.2175999</v>
+      </c>
+      <c r="M25">
+        <v>-31.984705200000001</v>
+      </c>
+      <c r="N25">
+        <v>-13.4595447</v>
+      </c>
+      <c r="O25">
+        <v>-30.2985352</v>
+      </c>
+      <c r="P25">
+        <v>-14.109465500000001</v>
+      </c>
+      <c r="Q25">
+        <v>-19.196473399999999</v>
+      </c>
+      <c r="R25">
+        <v>-16.701698100000002</v>
+      </c>
+      <c r="S25" s="3">
+        <f>AVERAGE(L25:R25)</f>
+        <v>-20.566860285714288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>-20.381800500000001</v>
@@ -1297,22 +2093,53 @@
         <v>-14.7327732</v>
       </c>
       <c r="E26">
+        <v>-14.506357700000001</v>
+      </c>
+      <c r="F26">
         <v>-13.7929718</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>-25.966559100000001</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>-17.677706400000002</v>
       </c>
-      <c r="H26" s="3">
-        <f t="shared" si="0"/>
-        <v>-19.31470271666667</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="3">
+        <f>AVERAGE(B26:H26)</f>
+        <v>-18.627796285714286</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26">
+        <v>-17.294701199999999</v>
+      </c>
+      <c r="M26">
+        <v>-30.4916464</v>
+      </c>
+      <c r="N26">
+        <v>-12.6093098</v>
+      </c>
+      <c r="O26">
+        <v>-23.0112609</v>
+      </c>
+      <c r="P26">
+        <v>-9.8376903999999996</v>
+      </c>
+      <c r="Q26">
+        <v>-10.601813699999999</v>
+      </c>
+      <c r="R26">
+        <v>-14.606989</v>
+      </c>
+      <c r="S26" s="3">
+        <f>AVERAGE(L26:R26)</f>
+        <v>-16.921915914285712</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>-21.835591999999998</v>
@@ -1324,22 +2151,53 @@
         <v>-13.203061</v>
       </c>
       <c r="E27">
+        <v>-9.5199739999999995</v>
+      </c>
+      <c r="F27">
         <v>-15.570838999999999</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>-4.9544290000000002</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>-18.15232</v>
       </c>
-      <c r="H27" s="3">
-        <f t="shared" si="0"/>
-        <v>-15.565160499999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="3">
+        <f>AVERAGE(B27:H27)</f>
+        <v>-14.701562428571426</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>-17.2872588</v>
+      </c>
+      <c r="M27">
+        <v>-36.854616399999998</v>
+      </c>
+      <c r="N27">
+        <v>-11.5675398</v>
+      </c>
+      <c r="O27">
+        <v>-24.689225</v>
+      </c>
+      <c r="P27">
+        <v>-12.2167098</v>
+      </c>
+      <c r="Q27">
+        <v>-15.1419671</v>
+      </c>
+      <c r="R27">
+        <v>-13.018887899999999</v>
+      </c>
+      <c r="S27" s="3">
+        <f>AVERAGE(L27:R27)</f>
+        <v>-18.682314971428575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>-17.024256900000001</v>
@@ -1351,22 +2209,53 @@
         <v>-12.6528718</v>
       </c>
       <c r="E28">
+        <v>-24.942329300000001</v>
+      </c>
+      <c r="F28">
         <v>-9.3788943000000007</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>-15.357067499999999</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>-11.964216800000001</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.023609333333333</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="3">
+        <f>AVERAGE(B28:H28)</f>
+        <v>-18.154855042857143</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28">
+        <v>-17.250018699999998</v>
+      </c>
+      <c r="M28">
+        <v>-31.888963799999999</v>
+      </c>
+      <c r="N28">
+        <v>-14.0132931</v>
+      </c>
+      <c r="O28">
+        <v>-17.640318300000001</v>
+      </c>
+      <c r="P28">
+        <v>-14.982514200000001</v>
+      </c>
+      <c r="Q28">
+        <v>-12.2655283</v>
+      </c>
+      <c r="R28">
+        <v>-18.328409300000001</v>
+      </c>
+      <c r="S28" s="3">
+        <f>AVERAGE(L28:R28)</f>
+        <v>-18.052720814285713</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>-21.051254400000001</v>
@@ -1378,22 +2267,53 @@
         <v>-14.488807400000001</v>
       </c>
       <c r="E29">
+        <v>-25.819765799999999</v>
+      </c>
+      <c r="F29">
         <v>-15.7279968</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>-21.044934699999999</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>-20.655329399999999</v>
       </c>
-      <c r="H29" s="3">
-        <f t="shared" si="0"/>
-        <v>-21.473784583333337</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="3">
+        <f>AVERAGE(B29:H29)</f>
+        <v>-22.094639042857146</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29">
+        <v>-17.071313199999999</v>
+      </c>
+      <c r="M29">
+        <v>-31.956562300000002</v>
+      </c>
+      <c r="N29">
+        <v>-13.4470721</v>
+      </c>
+      <c r="O29">
+        <v>-18.5957328</v>
+      </c>
+      <c r="P29">
+        <v>-13.079902499999999</v>
+      </c>
+      <c r="Q29">
+        <v>-13.011406300000001</v>
+      </c>
+      <c r="R29">
+        <v>-14.4059046</v>
+      </c>
+      <c r="S29" s="3">
+        <f>AVERAGE(L29:R29)</f>
+        <v>-17.366841971428574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>-23.006976300000002</v>
@@ -1405,22 +2325,53 @@
         <v>-12.8687497</v>
       </c>
       <c r="E30">
+        <v>-25.025856900000001</v>
+      </c>
+      <c r="F30">
         <v>-12.707176199999999</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>-16.2397293</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>-15.251213099999999</v>
       </c>
-      <c r="H30" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.544297583333332</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I30" s="3">
+        <f>AVERAGE(B30:H30)</f>
+        <v>-18.613091771428572</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30">
+        <v>-17.024256900000001</v>
+      </c>
+      <c r="M30">
+        <v>-35.764348699999999</v>
+      </c>
+      <c r="N30">
+        <v>-12.6528718</v>
+      </c>
+      <c r="O30">
+        <v>-24.942329300000001</v>
+      </c>
+      <c r="P30">
+        <v>-9.3788943000000007</v>
+      </c>
+      <c r="Q30">
+        <v>-15.357067499999999</v>
+      </c>
+      <c r="R30">
+        <v>-11.964216800000001</v>
+      </c>
+      <c r="S30" s="3">
+        <f>AVERAGE(L30:R30)</f>
+        <v>-18.154855042857143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>-19.459890300000001</v>
@@ -1432,22 +2383,53 @@
         <v>-13.967892600000001</v>
       </c>
       <c r="E31">
+        <v>-12.4247824</v>
+      </c>
+      <c r="F31">
         <v>-16.292657500000001</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>-8.9381845999999996</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>-18.078353199999999</v>
       </c>
-      <c r="H31" s="3">
-        <f t="shared" si="0"/>
-        <v>-17.119036949999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I31" s="3">
+        <f>AVERAGE(B31:H31)</f>
+        <v>-16.448429157142858</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31">
+        <v>-15.7261474</v>
+      </c>
+      <c r="M31">
+        <v>-27.276750199999999</v>
+      </c>
+      <c r="N31">
+        <v>-13.1792315</v>
+      </c>
+      <c r="O31">
+        <v>-24.939641999999999</v>
+      </c>
+      <c r="P31">
+        <v>-11.275166199999999</v>
+      </c>
+      <c r="Q31">
+        <v>-16.593104499999999</v>
+      </c>
+      <c r="R31">
+        <v>-15.2160967</v>
+      </c>
+      <c r="S31" s="3">
+        <f>AVERAGE(L31:R31)</f>
+        <v>-17.74373407142857</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>-24.278553299999999</v>
@@ -1459,21 +2441,152 @@
         <v>-14.940697200000001</v>
       </c>
       <c r="E32">
+        <v>-17.899998</v>
+      </c>
+      <c r="F32">
         <v>-19.242381999999999</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>-29.518176700000001</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>-22.701972999999999</v>
       </c>
-      <c r="H32" s="4">
-        <f t="shared" si="0"/>
-        <v>-22.44269846666667</v>
+      <c r="I32" s="4">
+        <f>AVERAGE(B32:H32)</f>
+        <v>-21.793741257142859</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32">
+        <v>-14.4346215</v>
+      </c>
+      <c r="M32">
+        <v>-36.946788300000001</v>
+      </c>
+      <c r="N32">
+        <v>-11.6185954</v>
+      </c>
+      <c r="O32">
+        <v>-26.387392500000001</v>
+      </c>
+      <c r="P32">
+        <v>-10.512088500000001</v>
+      </c>
+      <c r="Q32">
+        <v>-21.2859129</v>
+      </c>
+      <c r="R32">
+        <v>-12.835842599999999</v>
+      </c>
+      <c r="S32" s="4">
+        <f>AVERAGE(L32:R32)</f>
+        <v>-19.145891671428576</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B32">
+  <mergeCells count="2">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="L1:S1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:B32">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C32">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D32">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E32">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F32">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G32">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H32">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I32">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L32">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1485,7 +2598,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C32">
+  <conditionalFormatting sqref="M3:M32">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1497,7 +2610,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
+  <conditionalFormatting sqref="N3:N32">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1509,7 +2622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
+  <conditionalFormatting sqref="O3:O32">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1521,7 +2634,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
+  <conditionalFormatting sqref="P3:P32">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1533,7 +2646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
+  <conditionalFormatting sqref="Q3:Q32">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1545,8 +2658,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="R3:R32">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1557,8 +2670,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H1048576">
-    <cfRule type="colorScale" priority="69">
+  <conditionalFormatting sqref="S3:S32">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1576,29 +2689,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="29.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1617,16 +2765,46 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0.64</v>
@@ -1638,22 +2816,53 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="E3">
+        <v>-9.843</v>
+      </c>
+      <c r="F3">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>-1.766</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.85</v>
       </c>
-      <c r="H3" s="3">
-        <f>AVERAGE(B3:G3)</f>
-        <v>-0.33649999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="6">
+        <f>AVERAGE(B3:H3)</f>
+        <v>-1.6945714285714286</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="M3">
+        <v>-48.353000000000002</v>
+      </c>
+      <c r="N3">
+        <v>0.44</v>
+      </c>
+      <c r="O3">
+        <v>-34.415999999999997</v>
+      </c>
+      <c r="P3">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="R3">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="S3" s="6">
+        <f>AVERAGE(L3:R3)</f>
+        <v>-11.309428571428571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>-0.27600000000000002</v>
@@ -1665,22 +2874,53 @@
         <v>-1392.027</v>
       </c>
       <c r="E4">
+        <v>-13.678000000000001</v>
+      </c>
+      <c r="F4">
         <v>-1.044</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>-3.8540000000000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-7.6820000000000004</v>
       </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H32" si="0">AVERAGE(B4:G4)</f>
-        <v>-234.69433333333336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I32" si="0">AVERAGE(B4:H4)</f>
+        <v>-203.12057142857148</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="M4">
+        <v>-48.878</v>
+      </c>
+      <c r="N4">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="O4">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="Q4">
+        <v>-16.427</v>
+      </c>
+      <c r="R4">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="S4" s="3">
+        <f>AVERAGE(L4:R4)</f>
+        <v>-11.147428571428572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.502</v>
@@ -1692,22 +2932,53 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="E5">
+        <v>-11.425000000000001</v>
+      </c>
+      <c r="F5">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.69299999999999995</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>0.35516666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.3277142857142861</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="M5">
+        <v>-36.286999999999999</v>
+      </c>
+      <c r="N5">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="O5">
+        <v>-5.8650000000000002</v>
+      </c>
+      <c r="P5">
+        <v>-0.06</v>
+      </c>
+      <c r="Q5">
+        <v>-5.319</v>
+      </c>
+      <c r="R5">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="S5" s="3">
+        <f>AVERAGE(L5:R5)</f>
+        <v>-6.6317142857142866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0.34599999999999997</v>
@@ -1719,22 +2990,53 @@
         <v>-6.9000000000000006E-2</v>
       </c>
       <c r="E6">
+        <v>-3.0419999999999998</v>
+      </c>
+      <c r="F6">
         <v>-1.0760000000000001</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>-20.052</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.16900000000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>-4.3596666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-4.1714285714285717</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>0.755</v>
+      </c>
+      <c r="M6">
+        <v>-35.832999999999998</v>
+      </c>
+      <c r="N6">
+        <v>0.315</v>
+      </c>
+      <c r="O6">
+        <v>-15.010999999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="Q6">
+        <v>-15.532</v>
+      </c>
+      <c r="R6">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="S6" s="3">
+        <f>AVERAGE(L6:R6)</f>
+        <v>-9.2214285714285715</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0.158</v>
@@ -1746,22 +3048,53 @@
         <v>-0.218</v>
       </c>
       <c r="E7">
+        <v>-6.4180000000000001</v>
+      </c>
+      <c r="F7">
         <v>-0.187</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>-7.1369999999999996</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-0.27300000000000002</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>-1.5333333333333332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-2.2311428571428569</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7">
+        <v>0.71</v>
+      </c>
+      <c r="M7">
+        <v>-3.0840000000000001</v>
+      </c>
+      <c r="N7">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O7">
+        <v>-2.786</v>
+      </c>
+      <c r="P7">
+        <v>0.115</v>
+      </c>
+      <c r="Q7">
+        <v>-3.9550000000000001</v>
+      </c>
+      <c r="R7">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="S7" s="3">
+        <f>AVERAGE(L7:R7)</f>
+        <v>-1.2062857142857144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.63400000000000001</v>
@@ -1773,22 +3106,53 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="E8">
+        <v>-1.056</v>
+      </c>
+      <c r="F8">
         <v>0.73199999999999998</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>-6.5330000000000004</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.80500000000000005</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>-0.64316666666666678</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-0.70214285714285729</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M8">
+        <v>-131.82499999999999</v>
+      </c>
+      <c r="N8">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="O8">
+        <v>-242.89599999999999</v>
+      </c>
+      <c r="P8">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>-83.959000000000003</v>
+      </c>
+      <c r="R8">
+        <v>0.61</v>
+      </c>
+      <c r="S8" s="3">
+        <f>AVERAGE(L8:R8)</f>
+        <v>-65.249999999999986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>-0.625</v>
@@ -1800,22 +3164,53 @@
         <v>-0.20399999999999999</v>
       </c>
       <c r="E9">
+        <v>-4.0170000000000003</v>
+      </c>
+      <c r="F9">
         <v>-0.75700000000000001</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>-0.97699999999999998</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>-0.32800000000000001</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>-0.73000000000000009</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.1995714285714285</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="M9">
+        <v>-123.502</v>
+      </c>
+      <c r="N9">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="O9">
+        <v>-250.1</v>
+      </c>
+      <c r="P9">
+        <v>-0.95699999999999996</v>
+      </c>
+      <c r="Q9">
+        <v>-34.518999999999998</v>
+      </c>
+      <c r="R9">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="S9" s="3">
+        <f>AVERAGE(L9:R9)</f>
+        <v>-58.205714285714286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>0.32</v>
@@ -1827,22 +3222,53 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="E10">
+        <v>-1.0389999999999999</v>
+      </c>
+      <c r="F10">
         <v>0.23200000000000001</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-2.1989999999999998</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.45500000000000002</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>-1.2971666666666666</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.2602857142857142</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="M10">
+        <v>-2.1859999999999999</v>
+      </c>
+      <c r="N10">
+        <v>0.378</v>
+      </c>
+      <c r="O10">
+        <v>-4.718</v>
+      </c>
+      <c r="P10">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="Q10">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="R10">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="S10" s="3">
+        <f>AVERAGE(L10:R10)</f>
+        <v>-0.81685714285714284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>0.15</v>
@@ -1854,22 +3280,53 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="E11">
+        <v>-36.598999999999997</v>
+      </c>
+      <c r="F11">
         <v>0.372</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>-14.78</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.625</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>-3.3839999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-8.1289999999999996</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="M11">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="N11">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="O11">
+        <v>-8.952</v>
+      </c>
+      <c r="P11">
+        <v>0.124</v>
+      </c>
+      <c r="Q11">
+        <v>-1.091</v>
+      </c>
+      <c r="R11">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="S11" s="3">
+        <f>AVERAGE(L11:R11)</f>
+        <v>-1.1084285714285713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -1881,22 +3338,53 @@
         <v>0.189</v>
       </c>
       <c r="E12">
+        <v>-0.51900000000000002</v>
+      </c>
+      <c r="F12">
         <v>0.24099999999999999</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-0.51800000000000002</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.44500000000000001</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>-6.1428333333333329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-5.339428571428571</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>0.64</v>
+      </c>
+      <c r="M12">
+        <v>-3.073</v>
+      </c>
+      <c r="N12">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="O12">
+        <v>-9.843</v>
+      </c>
+      <c r="P12">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="Q12">
+        <v>-1.766</v>
+      </c>
+      <c r="R12">
+        <v>0.85</v>
+      </c>
+      <c r="S12" s="3">
+        <f>AVERAGE(L12:R12)</f>
+        <v>-1.6945714285714286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>-0.20699999999999999</v>
@@ -1908,22 +3396,53 @@
         <v>0.16</v>
       </c>
       <c r="E13">
+        <v>-6.0019999999999998</v>
+      </c>
+      <c r="F13">
         <v>-0.47399999999999998</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>-4.8259999999999996</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.23200000000000001</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>-4.5311666666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-4.7412857142857145</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="M13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="N13">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="O13">
+        <v>-1.056</v>
+      </c>
+      <c r="P13">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="Q13">
+        <v>-6.5330000000000004</v>
+      </c>
+      <c r="R13">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="S13" s="3">
+        <f>AVERAGE(L13:R13)</f>
+        <v>-0.70214285714285729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.71</v>
@@ -1935,22 +3454,53 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="E14">
+        <v>-2.786</v>
+      </c>
+      <c r="F14">
         <v>0.115</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-3.9550000000000001</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.23400000000000001</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>-0.94300000000000006</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.2062857142857144</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="M14">
+        <v>-10.510999999999999</v>
+      </c>
+      <c r="N14">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="O14">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="P14">
+        <v>0.435</v>
+      </c>
+      <c r="Q14">
+        <v>-0.248</v>
+      </c>
+      <c r="R14">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="S14" s="3">
+        <f>AVERAGE(L14:R14)</f>
+        <v>-1.2234285714285711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0.755</v>
@@ -1962,22 +3512,53 @@
         <v>0.315</v>
       </c>
       <c r="E15">
+        <v>-15.010999999999999</v>
+      </c>
+      <c r="F15">
         <v>0.27400000000000002</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-15.532</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.48199999999999998</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>-8.2565000000000008</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-9.2214285714285715</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L15">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="M15">
+        <v>-0.60499999999999998</v>
+      </c>
+      <c r="N15">
+        <v>0.153</v>
+      </c>
+      <c r="O15">
+        <v>-1.746</v>
+      </c>
+      <c r="P15">
+        <v>-0.24399999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>-0.42699999999999999</v>
+      </c>
+      <c r="R15">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="S15" s="3">
+        <f>AVERAGE(L15:R15)</f>
+        <v>-0.23114285714285715</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>0.48899999999999999</v>
@@ -1989,22 +3570,53 @@
         <v>0.309</v>
       </c>
       <c r="E16">
+        <v>-620.23699999999997</v>
+      </c>
+      <c r="F16">
         <v>0.76</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>-15.16</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.76300000000000001</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <f t="shared" si="0"/>
-        <v>-12.105333333333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-98.981285714285704</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M16">
+        <v>-56.161999999999999</v>
+      </c>
+      <c r="N16">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="O16">
+        <v>-76.369</v>
+      </c>
+      <c r="P16">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="Q16">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="R16">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="S16" s="3">
+        <f>AVERAGE(L16:R16)</f>
+        <v>-18.638142857142856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0.59599999999999997</v>
@@ -2016,22 +3628,53 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="E17">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="F17">
         <v>0.435</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>-0.248</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.58199999999999996</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <f t="shared" si="0"/>
-        <v>-1.4669999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.2234285714285711</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="M17">
+        <v>-36.090000000000003</v>
+      </c>
+      <c r="N17">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="O17">
+        <v>-109.74299999999999</v>
+      </c>
+      <c r="P17">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>-28.056000000000001</v>
+      </c>
+      <c r="R17">
+        <v>0.4</v>
+      </c>
+      <c r="S17" s="3">
+        <f>AVERAGE(L17:R17)</f>
+        <v>-24.539571428571431</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>0.52300000000000002</v>
@@ -2043,22 +3686,53 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="E18">
+        <v>-6.68</v>
+      </c>
+      <c r="F18">
         <v>-1.909</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>-14.901</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.46500000000000002</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <f t="shared" si="0"/>
-        <v>-2.8013333333333335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-3.3554285714285714</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="M18">
+        <v>-1.123</v>
+      </c>
+      <c r="N18">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="O18">
+        <v>-6.68</v>
+      </c>
+      <c r="P18">
+        <v>-1.909</v>
+      </c>
+      <c r="Q18">
+        <v>-14.901</v>
+      </c>
+      <c r="R18">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="S18" s="3">
+        <f>AVERAGE(L18:R18)</f>
+        <v>-3.3554285714285714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>0.43099999999999999</v>
@@ -2070,22 +3744,53 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="E19">
+        <v>-2.7730000000000001</v>
+      </c>
+      <c r="F19">
         <v>-0.58799999999999997</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>-14.455</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0.28599999999999998</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <f t="shared" si="0"/>
-        <v>-2.6428333333333334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-2.6614285714285715</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>0.502</v>
+      </c>
+      <c r="M19">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="N19">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="O19">
+        <v>-11.425000000000001</v>
+      </c>
+      <c r="P19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q19">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="R19">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="S19" s="3">
+        <f>AVERAGE(L19:R19)</f>
+        <v>-1.3277142857142861</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>0.68700000000000006</v>
@@ -2097,22 +3802,53 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="E20">
+        <v>-250.1</v>
+      </c>
+      <c r="F20">
         <v>-0.95699999999999996</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>-34.518999999999998</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>0.65700000000000003</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <f t="shared" si="0"/>
-        <v>-26.223333333333329</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-58.205714285714286</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20">
+        <v>0.5</v>
+      </c>
+      <c r="M20">
+        <v>-37.713999999999999</v>
+      </c>
+      <c r="N20">
+        <v>0.189</v>
+      </c>
+      <c r="O20">
+        <v>-0.51900000000000002</v>
+      </c>
+      <c r="P20">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>-0.51800000000000002</v>
+      </c>
+      <c r="R20">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="S20" s="3">
+        <f>AVERAGE(L20:R20)</f>
+        <v>-5.339428571428571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0.64100000000000001</v>
@@ -2124,22 +3860,53 @@
         <v>0.39100000000000001</v>
       </c>
       <c r="E21">
+        <v>-8.952</v>
+      </c>
+      <c r="F21">
         <v>0.124</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>-1.091</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>0.71899999999999997</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <f t="shared" si="0"/>
-        <v>0.19883333333333333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-1.1084285714285713</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="M21">
+        <v>-59.792999999999999</v>
+      </c>
+      <c r="N21">
+        <v>0.309</v>
+      </c>
+      <c r="O21">
+        <v>-620.23699999999997</v>
+      </c>
+      <c r="P21">
+        <v>0.76</v>
+      </c>
+      <c r="Q21">
+        <v>-15.16</v>
+      </c>
+      <c r="R21">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="S21" s="3">
+        <f>AVERAGE(L21:R21)</f>
+        <v>-98.981285714285704</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0.115</v>
@@ -2151,22 +3918,53 @@
         <v>0.21</v>
       </c>
       <c r="E22">
+        <v>-29.173999999999999</v>
+      </c>
+      <c r="F22">
         <v>2.7E-2</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>-12.29</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <f t="shared" si="0"/>
-        <v>-3.1194999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-6.8415714285714282</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="M22">
+        <v>-30.119</v>
+      </c>
+      <c r="N22">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="O22">
+        <v>-123.947</v>
+      </c>
+      <c r="P22">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="Q22">
+        <v>-32.948999999999998</v>
+      </c>
+      <c r="R22">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="S22" s="3">
+        <f>AVERAGE(L22:R22)</f>
+        <v>-26.441142857142854</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0.82599999999999996</v>
@@ -2178,22 +3976,53 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="E23">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="F23">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>-16.427</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0.89600000000000002</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <f t="shared" si="0"/>
-        <v>-10.367833333333333</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-11.147428571428572</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="M23">
+        <v>-1.569</v>
+      </c>
+      <c r="N23">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="O23">
+        <v>-2.7730000000000001</v>
+      </c>
+      <c r="P23">
+        <v>-0.58799999999999997</v>
+      </c>
+      <c r="Q23">
+        <v>-14.455</v>
+      </c>
+      <c r="R23">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="S23" s="3">
+        <f>AVERAGE(L23:R23)</f>
+        <v>-2.6614285714285715</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0.59199999999999997</v>
@@ -2205,22 +4034,53 @@
         <v>0.153</v>
       </c>
       <c r="E24">
+        <v>-1.746</v>
+      </c>
+      <c r="F24">
         <v>-0.24399999999999999</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>-0.42699999999999999</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.65900000000000003</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <f t="shared" si="0"/>
-        <v>2.1333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-0.23114285714285715</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="M24">
+        <v>-5.476</v>
+      </c>
+      <c r="N24">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="O24">
+        <v>-3.0419999999999998</v>
+      </c>
+      <c r="P24">
+        <v>-1.0760000000000001</v>
+      </c>
+      <c r="Q24">
+        <v>-20.052</v>
+      </c>
+      <c r="R24">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="S24" s="3">
+        <f>AVERAGE(L24:R24)</f>
+        <v>-4.1714285714285717</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>0.55200000000000005</v>
@@ -2232,22 +4092,53 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="E25">
+        <v>-109.74299999999999</v>
+      </c>
+      <c r="F25">
         <v>0.76500000000000001</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>-28.056000000000001</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>0.4</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <f t="shared" si="0"/>
-        <v>-10.339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-24.539571428571431</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25">
+        <v>0.32</v>
+      </c>
+      <c r="M25">
+        <v>-6.8029999999999999</v>
+      </c>
+      <c r="N25">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="O25">
+        <v>-1.0389999999999999</v>
+      </c>
+      <c r="P25">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="Q25">
+        <v>-2.1989999999999998</v>
+      </c>
+      <c r="R25">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="S25" s="3">
+        <f>AVERAGE(L25:R25)</f>
+        <v>-1.2602857142857142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>0.58699999999999997</v>
@@ -2259,22 +4150,53 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="E26">
+        <v>-76.369</v>
+      </c>
+      <c r="F26">
         <v>0.17399999999999999</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0.32700000000000001</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>0.56399999999999995</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <f t="shared" si="0"/>
-        <v>-9.0163333333333338</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-18.638142857142856</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26">
+        <v>0.158</v>
+      </c>
+      <c r="M26">
+        <v>-1.5429999999999999</v>
+      </c>
+      <c r="N26">
+        <v>-0.218</v>
+      </c>
+      <c r="O26">
+        <v>-6.4180000000000001</v>
+      </c>
+      <c r="P26">
+        <v>-0.187</v>
+      </c>
+      <c r="Q26">
+        <v>-7.1369999999999996</v>
+      </c>
+      <c r="R26">
+        <v>-0.27300000000000002</v>
+      </c>
+      <c r="S26" s="3">
+        <f>AVERAGE(L26:R26)</f>
+        <v>-2.2311428571428569</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>0.70399999999999996</v>
@@ -2286,22 +4208,53 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="E27">
+        <v>-242.89599999999999</v>
+      </c>
+      <c r="F27">
         <v>0.45200000000000001</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>-83.959000000000003</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>0.61</v>
       </c>
-      <c r="H27" s="3">
+      <c r="I27" s="3">
         <f t="shared" si="0"/>
-        <v>-35.642333333333333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-65.249999999999986</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27">
+        <v>0.15</v>
+      </c>
+      <c r="M27">
+        <v>-6.9770000000000003</v>
+      </c>
+      <c r="N27">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="O27">
+        <v>-36.598999999999997</v>
+      </c>
+      <c r="P27">
+        <v>0.372</v>
+      </c>
+      <c r="Q27">
+        <v>-14.78</v>
+      </c>
+      <c r="R27">
+        <v>0.625</v>
+      </c>
+      <c r="S27" s="3">
+        <f>AVERAGE(L27:R27)</f>
+        <v>-8.1289999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>0.105</v>
@@ -2313,22 +4266,53 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E28">
+        <v>-5.9980000000000002</v>
+      </c>
+      <c r="F28">
         <v>-1.2809999999999999</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>-6.7439999999999998</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>-0.623</v>
       </c>
-      <c r="H28" s="3">
+      <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>-1.7933333333333332</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-2.3939999999999997</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28">
+        <v>0.115</v>
+      </c>
+      <c r="M28">
+        <v>-6.8540000000000001</v>
+      </c>
+      <c r="N28">
+        <v>0.21</v>
+      </c>
+      <c r="O28">
+        <v>-29.173999999999999</v>
+      </c>
+      <c r="P28">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Q28">
+        <v>-12.29</v>
+      </c>
+      <c r="R28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="S28" s="3">
+        <f>AVERAGE(L28:R28)</f>
+        <v>-6.8415714285714282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>0.64600000000000002</v>
@@ -2340,22 +4324,53 @@
         <v>0.378</v>
       </c>
       <c r="E29">
+        <v>-4.718</v>
+      </c>
+      <c r="F29">
         <v>0.47099999999999997</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>-1.0900000000000001</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>0.78100000000000003</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <f t="shared" si="0"/>
-        <v>-0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-0.81685714285714284</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29">
+        <v>0.105</v>
+      </c>
+      <c r="M29">
+        <v>-2.2679999999999998</v>
+      </c>
+      <c r="N29">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O29">
+        <v>-5.9980000000000002</v>
+      </c>
+      <c r="P29">
+        <v>-1.2809999999999999</v>
+      </c>
+      <c r="Q29">
+        <v>-6.7439999999999998</v>
+      </c>
+      <c r="R29">
+        <v>-0.623</v>
+      </c>
+      <c r="S29" s="3">
+        <f>AVERAGE(L29:R29)</f>
+        <v>-2.3939999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>0.77400000000000002</v>
@@ -2367,22 +4382,53 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="E30">
+        <v>-5.8650000000000002</v>
+      </c>
+      <c r="F30">
         <v>-0.06</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>-5.319</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <f t="shared" si="0"/>
-        <v>-6.7595000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-6.6317142857142866</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="M30">
+        <v>-22.071999999999999</v>
+      </c>
+      <c r="N30">
+        <v>0.16</v>
+      </c>
+      <c r="O30">
+        <v>-6.0019999999999998</v>
+      </c>
+      <c r="P30">
+        <v>-0.47399999999999998</v>
+      </c>
+      <c r="Q30">
+        <v>-4.8259999999999996</v>
+      </c>
+      <c r="R30">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="S30" s="3">
+        <f>AVERAGE(L30:R30)</f>
+        <v>-4.7412857142857145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>0.48899999999999999</v>
@@ -2394,22 +4440,53 @@
         <v>0.29899999999999999</v>
       </c>
       <c r="E31">
+        <v>-123.947</v>
+      </c>
+      <c r="F31">
         <v>0.53600000000000003</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>-32.948999999999998</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>0.60299999999999998</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <f t="shared" si="0"/>
-        <v>-10.190166666666666</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>-26.441142857142854</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31">
+        <v>-0.27600000000000002</v>
+      </c>
+      <c r="M31">
+        <v>-3.2829999999999999</v>
+      </c>
+      <c r="N31">
+        <v>-1392.027</v>
+      </c>
+      <c r="O31">
+        <v>-13.678000000000001</v>
+      </c>
+      <c r="P31">
+        <v>-1.044</v>
+      </c>
+      <c r="Q31">
+        <v>-3.8540000000000001</v>
+      </c>
+      <c r="R31">
+        <v>-7.6820000000000004</v>
+      </c>
+      <c r="S31" s="3">
+        <f>AVERAGE(L31:R31)</f>
+        <v>-203.12057142857148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>0.83199999999999996</v>
@@ -2421,321 +4498,193 @@
         <v>0.44</v>
       </c>
       <c r="E32">
+        <v>-34.415999999999997</v>
+      </c>
+      <c r="F32">
         <v>0.76500000000000001</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>0.70299999999999996</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>0.86299999999999999</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="4">
         <f t="shared" si="0"/>
-        <v>-7.458333333333333</v>
+        <v>-11.309428571428571</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32">
+        <v>-0.625</v>
+      </c>
+      <c r="M32">
+        <v>-1.4890000000000001</v>
+      </c>
+      <c r="N32">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="O32">
+        <v>-4.0170000000000003</v>
+      </c>
+      <c r="P32">
+        <v>-0.75700000000000001</v>
+      </c>
+      <c r="Q32">
+        <v>-0.97699999999999998</v>
+      </c>
+      <c r="R32">
+        <v>-0.32800000000000001</v>
+      </c>
+      <c r="S32" s="4">
+        <f>AVERAGE(L32:R32)</f>
+        <v>-1.1995714285714285</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K2:S32" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K3:S32">
+      <sortCondition descending="1" ref="L2:L32"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="2">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="L1:S1"/>
+  </mergeCells>
   <conditionalFormatting sqref="B3:B32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C32">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="30"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C32">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="20"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D32">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E32">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F32">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D32">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="44">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G32">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="45">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H32">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E32">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="40">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I32">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="41">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L32">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F32">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="36">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M32">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="37">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N32">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G32">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H32">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS(B+$B$3:$B$32-1))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32-1))"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="formula" val="&quot;MIN(ABS($B$2:$B$31))&quot;"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="&quot;MAX(ABS($B$2:$B$31))&quot;"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="formula" val="MIN(ABS($B$3:$B$32))"/>
-        <cfvo type="formula" val="MAX(ABS($B$3:$B$32))"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
+  <conditionalFormatting sqref="O3:O32">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2747,19 +4696,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
+  <conditionalFormatting sqref="P3:P32">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2771,7 +4708,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
+  <conditionalFormatting sqref="Q3:Q32">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2783,7 +4720,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1048576">
+  <conditionalFormatting sqref="R3:R32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2795,7 +4732,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
+  <conditionalFormatting sqref="S3:S32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Autoformer results finished and sent
</commit_message>
<xml_diff>
--- a/TFG_Results/Transformer_results/Transformer_metrics.xlsx
+++ b/TFG_Results/Transformer_results/Transformer_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\OneDrive\Escritorio\TFG_TST\TFG_Results\Transformer_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01002F6-07AE-43C1-8DEB-E469E8F0C376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CFCEF1-E6F0-435D-817F-34B032C76853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2610" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -320,10 +320,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -332,6 +328,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,33 +669,33 @@
     <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="K1" s="7" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -714,7 +722,7 @@
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -741,7 +749,7 @@
       <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -771,7 +779,7 @@
         <v>-22.3636421</v>
       </c>
       <c r="I3" s="3">
-        <f>AVERAGE(B3:H3)</f>
+        <f t="shared" ref="I3:I32" si="0">AVERAGE(B3:H3)</f>
         <v>-23.413513185714287</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -799,7 +807,7 @@
         <v>-22.701972999999999</v>
       </c>
       <c r="S3" s="3">
-        <f>AVERAGE(L3:R3)</f>
+        <f t="shared" ref="S3:S32" si="1">AVERAGE(L3:R3)</f>
         <v>-21.793741257142859</v>
       </c>
     </row>
@@ -829,7 +837,7 @@
         <v>-18.658907200000002</v>
       </c>
       <c r="I4" s="3">
-        <f>AVERAGE(B4:H4)</f>
+        <f t="shared" si="0"/>
         <v>-24.804781114285714</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -857,7 +865,7 @@
         <v>-23.898673800000001</v>
       </c>
       <c r="S4" s="3">
-        <f>AVERAGE(L4:R4)</f>
+        <f t="shared" si="1"/>
         <v>-20.275888342857144</v>
       </c>
     </row>
@@ -887,7 +895,7 @@
         <v>-19.191879</v>
       </c>
       <c r="I5" s="3">
-        <f>AVERAGE(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>-22.360817071428574</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -915,7 +923,7 @@
         <v>-15.251213099999999</v>
       </c>
       <c r="S5" s="3">
-        <f>AVERAGE(L5:R5)</f>
+        <f t="shared" si="1"/>
         <v>-18.613091771428572</v>
       </c>
     </row>
@@ -945,7 +953,7 @@
         <v>-14.606989</v>
       </c>
       <c r="I6" s="3">
-        <f>AVERAGE(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>-16.921915914285712</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -973,7 +981,7 @@
         <v>-16.922112500000001</v>
       </c>
       <c r="S6" s="3">
-        <f>AVERAGE(L6:R6)</f>
+        <f t="shared" si="1"/>
         <v>-18.092339857142857</v>
       </c>
     </row>
@@ -1003,7 +1011,7 @@
         <v>-13.018887899999999</v>
       </c>
       <c r="I7" s="3">
-        <f>AVERAGE(B7:H7)</f>
+        <f t="shared" si="0"/>
         <v>-18.682314971428575</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1031,7 +1039,7 @@
         <v>-15.225873399999999</v>
       </c>
       <c r="S7" s="3">
-        <f>AVERAGE(L7:R7)</f>
+        <f t="shared" si="1"/>
         <v>-20.635341614285718</v>
       </c>
     </row>
@@ -1061,7 +1069,7 @@
         <v>-21.170314000000001</v>
       </c>
       <c r="I8" s="3">
-        <f>AVERAGE(B8:H8)</f>
+        <f t="shared" si="0"/>
         <v>-23.206185285714287</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1089,7 +1097,7 @@
         <v>-18.15232</v>
       </c>
       <c r="S8" s="3">
-        <f>AVERAGE(L8:R8)</f>
+        <f t="shared" si="1"/>
         <v>-14.701562428571426</v>
       </c>
     </row>
@@ -1119,7 +1127,7 @@
         <v>-12.835842599999999</v>
       </c>
       <c r="I9" s="3">
-        <f>AVERAGE(B9:H9)</f>
+        <f t="shared" si="0"/>
         <v>-19.145891671428576</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1147,7 +1155,7 @@
         <v>-18.710442499999999</v>
       </c>
       <c r="S9" s="3">
-        <f>AVERAGE(L9:R9)</f>
+        <f t="shared" si="1"/>
         <v>-14.623053885714286</v>
       </c>
     </row>
@@ -1177,7 +1185,7 @@
         <v>-16.701698100000002</v>
       </c>
       <c r="I10" s="3">
-        <f>AVERAGE(B10:H10)</f>
+        <f t="shared" si="0"/>
         <v>-20.566860285714288</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1205,7 +1213,7 @@
         <v>-20.655329399999999</v>
       </c>
       <c r="S10" s="3">
-        <f>AVERAGE(L10:R10)</f>
+        <f t="shared" si="1"/>
         <v>-22.094639042857146</v>
       </c>
     </row>
@@ -1235,7 +1243,7 @@
         <v>-18.328409300000001</v>
       </c>
       <c r="I11" s="3">
-        <f>AVERAGE(B11:H11)</f>
+        <f t="shared" si="0"/>
         <v>-18.052720814285713</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1263,7 +1271,7 @@
         <v>-22.3636421</v>
       </c>
       <c r="S11" s="3">
-        <f>AVERAGE(L11:R11)</f>
+        <f t="shared" si="1"/>
         <v>-23.413513185714287</v>
       </c>
     </row>
@@ -1293,7 +1301,7 @@
         <v>-16.625015600000001</v>
       </c>
       <c r="I12" s="3">
-        <f>AVERAGE(B12:H12)</f>
+        <f t="shared" si="0"/>
         <v>-20.387684385714287</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1321,7 +1329,7 @@
         <v>-19.5807295</v>
       </c>
       <c r="S12" s="3">
-        <f>AVERAGE(L12:R12)</f>
+        <f t="shared" si="1"/>
         <v>-22.333221685714285</v>
       </c>
     </row>
@@ -1351,7 +1359,7 @@
         <v>-15.2160967</v>
       </c>
       <c r="I13" s="3">
-        <f>AVERAGE(B13:H13)</f>
+        <f t="shared" si="0"/>
         <v>-17.74373407142857</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -1379,7 +1387,7 @@
         <v>-21.170314000000001</v>
       </c>
       <c r="S13" s="3">
-        <f>AVERAGE(L13:R13)</f>
+        <f t="shared" si="1"/>
         <v>-23.206185285714287</v>
       </c>
     </row>
@@ -1409,7 +1417,7 @@
         <v>-15.225873399999999</v>
       </c>
       <c r="I14" s="3">
-        <f>AVERAGE(B14:H14)</f>
+        <f t="shared" si="0"/>
         <v>-20.635341614285718</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -1437,7 +1445,7 @@
         <v>-17.853883700000001</v>
       </c>
       <c r="S14" s="3">
-        <f>AVERAGE(L14:R14)</f>
+        <f t="shared" si="1"/>
         <v>-22.310282614285715</v>
       </c>
     </row>
@@ -1467,7 +1475,7 @@
         <v>-16.922112500000001</v>
       </c>
       <c r="I15" s="3">
-        <f>AVERAGE(B15:H15)</f>
+        <f t="shared" si="0"/>
         <v>-18.092339857142857</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -1495,7 +1503,7 @@
         <v>-18.745516299999998</v>
       </c>
       <c r="S15" s="3">
-        <f>AVERAGE(L15:R15)</f>
+        <f t="shared" si="1"/>
         <v>-22.128156271428569</v>
       </c>
     </row>
@@ -1525,7 +1533,7 @@
         <v>-20.3138197</v>
       </c>
       <c r="I16" s="3">
-        <f>AVERAGE(B16:H16)</f>
+        <f t="shared" si="0"/>
         <v>-16.234625814285714</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -1553,7 +1561,7 @@
         <v>-18.658907200000002</v>
       </c>
       <c r="S16" s="3">
-        <f>AVERAGE(L16:R16)</f>
+        <f t="shared" si="1"/>
         <v>-24.804781114285714</v>
       </c>
     </row>
@@ -1583,7 +1591,7 @@
         <v>-17.853883700000001</v>
       </c>
       <c r="I17" s="3">
-        <f>AVERAGE(B17:H17)</f>
+        <f t="shared" si="0"/>
         <v>-22.310282614285715</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1611,7 +1619,7 @@
         <v>-17.677706400000002</v>
       </c>
       <c r="S17" s="3">
-        <f>AVERAGE(L17:R17)</f>
+        <f t="shared" si="1"/>
         <v>-18.627796285714286</v>
       </c>
     </row>
@@ -1641,7 +1649,7 @@
         <v>-16.7883104</v>
       </c>
       <c r="I18" s="3">
-        <f>AVERAGE(B18:H18)</f>
+        <f t="shared" si="0"/>
         <v>-18.905678014285716</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -1669,7 +1677,7 @@
         <v>-16.289753099999999</v>
       </c>
       <c r="S18" s="3">
-        <f>AVERAGE(L18:R18)</f>
+        <f t="shared" si="1"/>
         <v>-16.850179071428574</v>
       </c>
     </row>
@@ -1699,7 +1707,7 @@
         <v>-15.5308291</v>
       </c>
       <c r="I19" s="3">
-        <f>AVERAGE(B19:H19)</f>
+        <f t="shared" si="0"/>
         <v>-19.264973014285715</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -1727,7 +1735,7 @@
         <v>-16.7883104</v>
       </c>
       <c r="S19" s="3">
-        <f>AVERAGE(L19:R19)</f>
+        <f t="shared" si="1"/>
         <v>-18.905678014285716</v>
       </c>
     </row>
@@ -1757,7 +1765,7 @@
         <v>-18.710442499999999</v>
       </c>
       <c r="I20" s="3">
-        <f>AVERAGE(B20:H20)</f>
+        <f t="shared" si="0"/>
         <v>-14.623053885714286</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -1785,7 +1793,7 @@
         <v>-19.191879</v>
       </c>
       <c r="S20" s="3">
-        <f>AVERAGE(L20:R20)</f>
+        <f t="shared" si="1"/>
         <v>-22.360817071428574</v>
       </c>
     </row>
@@ -1815,7 +1823,7 @@
         <v>-19.5807295</v>
       </c>
       <c r="I21" s="3">
-        <f>AVERAGE(B21:H21)</f>
+        <f t="shared" si="0"/>
         <v>-22.333221685714285</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -1843,7 +1851,7 @@
         <v>-16.625015600000001</v>
       </c>
       <c r="S21" s="3">
-        <f>AVERAGE(L21:R21)</f>
+        <f t="shared" si="1"/>
         <v>-20.387684385714287</v>
       </c>
     </row>
@@ -1873,7 +1881,7 @@
         <v>-14.4059046</v>
       </c>
       <c r="I22" s="3">
-        <f>AVERAGE(B22:H22)</f>
+        <f t="shared" si="0"/>
         <v>-17.366841971428574</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -1901,7 +1909,7 @@
         <v>-20.3138197</v>
       </c>
       <c r="S22" s="3">
-        <f>AVERAGE(L22:R22)</f>
+        <f t="shared" si="1"/>
         <v>-16.234625814285714</v>
       </c>
     </row>
@@ -1931,7 +1939,7 @@
         <v>-23.898673800000001</v>
       </c>
       <c r="I23" s="3">
-        <f>AVERAGE(B23:H23)</f>
+        <f t="shared" si="0"/>
         <v>-20.275888342857144</v>
       </c>
       <c r="K23" s="1" t="s">
@@ -1959,7 +1967,7 @@
         <v>-18.078353199999999</v>
       </c>
       <c r="S23" s="3">
-        <f>AVERAGE(L23:R23)</f>
+        <f t="shared" si="1"/>
         <v>-16.448429157142858</v>
       </c>
     </row>
@@ -1989,7 +1997,7 @@
         <v>-18.745516299999998</v>
       </c>
       <c r="I24" s="3">
-        <f>AVERAGE(B24:H24)</f>
+        <f t="shared" si="0"/>
         <v>-22.128156271428569</v>
       </c>
       <c r="K24" s="1" t="s">
@@ -2017,7 +2025,7 @@
         <v>-15.5308291</v>
       </c>
       <c r="S24" s="3">
-        <f>AVERAGE(L24:R24)</f>
+        <f t="shared" si="1"/>
         <v>-19.264973014285715</v>
       </c>
     </row>
@@ -2047,7 +2055,7 @@
         <v>-16.289753099999999</v>
       </c>
       <c r="I25" s="3">
-        <f>AVERAGE(B25:H25)</f>
+        <f t="shared" si="0"/>
         <v>-16.850179071428574</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -2075,7 +2083,7 @@
         <v>-16.701698100000002</v>
       </c>
       <c r="S25" s="3">
-        <f>AVERAGE(L25:R25)</f>
+        <f t="shared" si="1"/>
         <v>-20.566860285714288</v>
       </c>
     </row>
@@ -2105,7 +2113,7 @@
         <v>-17.677706400000002</v>
       </c>
       <c r="I26" s="3">
-        <f>AVERAGE(B26:H26)</f>
+        <f t="shared" si="0"/>
         <v>-18.627796285714286</v>
       </c>
       <c r="K26" s="1" t="s">
@@ -2133,7 +2141,7 @@
         <v>-14.606989</v>
       </c>
       <c r="S26" s="3">
-        <f>AVERAGE(L26:R26)</f>
+        <f t="shared" si="1"/>
         <v>-16.921915914285712</v>
       </c>
     </row>
@@ -2163,7 +2171,7 @@
         <v>-18.15232</v>
       </c>
       <c r="I27" s="3">
-        <f>AVERAGE(B27:H27)</f>
+        <f t="shared" si="0"/>
         <v>-14.701562428571426</v>
       </c>
       <c r="K27" s="1" t="s">
@@ -2191,7 +2199,7 @@
         <v>-13.018887899999999</v>
       </c>
       <c r="S27" s="3">
-        <f>AVERAGE(L27:R27)</f>
+        <f t="shared" si="1"/>
         <v>-18.682314971428575</v>
       </c>
     </row>
@@ -2221,7 +2229,7 @@
         <v>-11.964216800000001</v>
       </c>
       <c r="I28" s="3">
-        <f>AVERAGE(B28:H28)</f>
+        <f t="shared" si="0"/>
         <v>-18.154855042857143</v>
       </c>
       <c r="K28" s="1" t="s">
@@ -2249,7 +2257,7 @@
         <v>-18.328409300000001</v>
       </c>
       <c r="S28" s="3">
-        <f>AVERAGE(L28:R28)</f>
+        <f t="shared" si="1"/>
         <v>-18.052720814285713</v>
       </c>
     </row>
@@ -2279,7 +2287,7 @@
         <v>-20.655329399999999</v>
       </c>
       <c r="I29" s="3">
-        <f>AVERAGE(B29:H29)</f>
+        <f t="shared" si="0"/>
         <v>-22.094639042857146</v>
       </c>
       <c r="K29" s="1" t="s">
@@ -2307,7 +2315,7 @@
         <v>-14.4059046</v>
       </c>
       <c r="S29" s="3">
-        <f>AVERAGE(L29:R29)</f>
+        <f t="shared" si="1"/>
         <v>-17.366841971428574</v>
       </c>
     </row>
@@ -2337,7 +2345,7 @@
         <v>-15.251213099999999</v>
       </c>
       <c r="I30" s="3">
-        <f>AVERAGE(B30:H30)</f>
+        <f t="shared" si="0"/>
         <v>-18.613091771428572</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -2365,7 +2373,7 @@
         <v>-11.964216800000001</v>
       </c>
       <c r="S30" s="3">
-        <f>AVERAGE(L30:R30)</f>
+        <f t="shared" si="1"/>
         <v>-18.154855042857143</v>
       </c>
     </row>
@@ -2395,7 +2403,7 @@
         <v>-18.078353199999999</v>
       </c>
       <c r="I31" s="3">
-        <f>AVERAGE(B31:H31)</f>
+        <f t="shared" si="0"/>
         <v>-16.448429157142858</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -2423,7 +2431,7 @@
         <v>-15.2160967</v>
       </c>
       <c r="S31" s="3">
-        <f>AVERAGE(L31:R31)</f>
+        <f t="shared" si="1"/>
         <v>-17.74373407142857</v>
       </c>
     </row>
@@ -2453,7 +2461,7 @@
         <v>-22.701972999999999</v>
       </c>
       <c r="I32" s="4">
-        <f>AVERAGE(B32:H32)</f>
+        <f t="shared" si="0"/>
         <v>-21.793741257142859</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -2481,7 +2489,7 @@
         <v>-12.835842599999999</v>
       </c>
       <c r="S32" s="4">
-        <f>AVERAGE(L32:R32)</f>
+        <f t="shared" si="1"/>
         <v>-19.145891671428576</v>
       </c>
     </row>
@@ -2691,1863 +2699,1859 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" customWidth="1"/>
-    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="K1" s="7" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>0.64</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>-3.073</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>0.48299999999999998</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>-9.843</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>0.84699999999999998</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>-1.766</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>0.85</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="9">
         <f>AVERAGE(B3:H3)</f>
         <v>-1.6945714285714286</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="6">
         <v>0.83199999999999996</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="6">
         <v>-48.353000000000002</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="6">
         <v>0.44</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="6">
         <v>-34.415999999999997</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="6">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="6">
         <v>0.70299999999999996</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="6">
         <v>0.86299999999999999</v>
       </c>
-      <c r="S3" s="6">
-        <f>AVERAGE(L3:R3)</f>
+      <c r="S3" s="9">
+        <f t="shared" ref="S3:S32" si="0">AVERAGE(L3:R3)</f>
         <v>-11.309428571428571</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>-0.27600000000000002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>-3.2829999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>-1392.027</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>-13.678000000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>-1.044</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>-3.8540000000000001</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <v>-7.6820000000000004</v>
       </c>
-      <c r="I4" s="3">
-        <f t="shared" ref="I4:I32" si="0">AVERAGE(B4:H4)</f>
+      <c r="I4" s="10">
+        <f t="shared" ref="I4:I32" si="1">AVERAGE(B4:H4)</f>
         <v>-203.12057142857148</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="6">
         <v>0.82599999999999996</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="6">
         <v>-48.878</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="6">
         <v>0.51900000000000002</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="6">
         <v>-15.824999999999999</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="6">
         <v>0.85699999999999998</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="6">
         <v>-16.427</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="6">
         <v>0.89600000000000002</v>
       </c>
-      <c r="S4" s="3">
-        <f>AVERAGE(L4:R4)</f>
+      <c r="S4" s="10">
+        <f t="shared" si="0"/>
         <v>-11.147428571428572</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>0.502</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.35899999999999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.20599999999999999</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>-11.425000000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" si="0"/>
+      <c r="I5" s="10">
+        <f t="shared" si="1"/>
         <v>-1.3277142857142861</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="6">
         <v>0.77400000000000002</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="6">
         <v>-36.286999999999999</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="6">
         <v>-5.8650000000000002</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="6">
         <v>-0.06</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="6">
         <v>-5.319</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="6">
         <v>0.23799999999999999</v>
       </c>
-      <c r="S5" s="3">
-        <f>AVERAGE(L5:R5)</f>
+      <c r="S5" s="10">
+        <f t="shared" si="0"/>
         <v>-6.6317142857142866</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>0.34599999999999997</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>-5.476</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>-6.9000000000000006E-2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>-3.0419999999999998</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>-1.0760000000000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>-20.052</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>0.16900000000000001</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="0"/>
+      <c r="I6" s="10">
+        <f t="shared" si="1"/>
         <v>-4.1714285714285717</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="6">
         <v>0.755</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="6">
         <v>-35.832999999999998</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="6">
         <v>0.315</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="6">
         <v>-15.010999999999999</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="6">
         <v>0.27400000000000002</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="6">
         <v>-15.532</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="6">
         <v>0.48199999999999998</v>
       </c>
-      <c r="S6" s="3">
-        <f>AVERAGE(L6:R6)</f>
+      <c r="S6" s="10">
+        <f t="shared" si="0"/>
         <v>-9.2214285714285715</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>0.158</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>-1.5429999999999999</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>-0.218</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>-6.4180000000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>-0.187</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>-7.1369999999999996</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>-0.27300000000000002</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="0"/>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
         <v>-2.2311428571428569</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="6">
         <v>0.71</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="6">
         <v>-3.0840000000000001</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="6">
         <v>0.32200000000000001</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="6">
         <v>-2.786</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="6">
         <v>0.115</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="6">
         <v>-3.9550000000000001</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="6">
         <v>0.23400000000000001</v>
       </c>
-      <c r="S7" s="3">
-        <f>AVERAGE(L7:R7)</f>
+      <c r="S7" s="10">
+        <f t="shared" si="0"/>
         <v>-1.2062857142857144</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>0.63400000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>0.14499999999999999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.35799999999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>-1.056</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>-6.5330000000000004</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>0.80500000000000005</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
         <v>-0.70214285714285729</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="6">
         <v>0.70399999999999996</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="6">
         <v>-131.82499999999999</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="6">
         <v>0.16400000000000001</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="6">
         <v>-242.89599999999999</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="6">
         <v>0.45200000000000001</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="6">
         <v>-83.959000000000003</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="6">
         <v>0.61</v>
       </c>
-      <c r="S8" s="3">
-        <f>AVERAGE(L8:R8)</f>
+      <c r="S8" s="10">
+        <f t="shared" si="0"/>
         <v>-65.249999999999986</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>-0.625</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>-1.4890000000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>-0.20399999999999999</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>-4.0170000000000003</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>-0.75700000000000001</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>-0.97699999999999998</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>-0.32800000000000001</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
         <v>-1.1995714285714285</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="6">
         <v>-123.502</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="6">
         <v>0.29399999999999998</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="6">
         <v>-250.1</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="6">
         <v>-0.95699999999999996</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="6">
         <v>-34.518999999999998</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="6">
         <v>0.65700000000000003</v>
       </c>
-      <c r="S9" s="3">
-        <f>AVERAGE(L9:R9)</f>
+      <c r="S9" s="10">
+        <f t="shared" si="0"/>
         <v>-58.205714285714286</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>0.32</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>-6.8029999999999999</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>0.21199999999999999</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>-1.0389999999999999</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>0.23200000000000001</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>-2.1989999999999998</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>0.45500000000000002</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
         <v>-1.2602857142857142</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <v>0.64600000000000002</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="6">
         <v>-2.1859999999999999</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="6">
         <v>0.378</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="6">
         <v>-4.718</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="6">
         <v>0.47099999999999997</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="6">
         <v>-1.0900000000000001</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="6">
         <v>0.78100000000000003</v>
       </c>
-      <c r="S10" s="3">
-        <f>AVERAGE(L10:R10)</f>
+      <c r="S10" s="10">
+        <f t="shared" si="0"/>
         <v>-0.81685714285714284</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>0.15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>-6.9770000000000003</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>-36.598999999999997</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>0.372</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>-14.78</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="6">
         <v>0.625</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
         <v>-8.1289999999999996</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="6">
         <v>0.64100000000000001</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="6">
         <v>0.40899999999999997</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="6">
         <v>0.39100000000000001</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="6">
         <v>-8.952</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="6">
         <v>0.124</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="6">
         <v>-1.091</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="6">
         <v>0.71899999999999997</v>
       </c>
-      <c r="S11" s="3">
-        <f>AVERAGE(L11:R11)</f>
+      <c r="S11" s="10">
+        <f t="shared" si="0"/>
         <v>-1.1084285714285713</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <v>0.5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>-37.713999999999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>0.189</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>-0.51900000000000002</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>0.24099999999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>-0.51800000000000002</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>0.44500000000000001</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="0"/>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
         <v>-5.339428571428571</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="6">
         <v>0.64</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="6">
         <v>-3.073</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="6">
         <v>0.48299999999999998</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="6">
         <v>-9.843</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="6">
         <v>0.84699999999999998</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="6">
         <v>-1.766</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="6">
         <v>0.85</v>
       </c>
-      <c r="S12" s="3">
-        <f>AVERAGE(L12:R12)</f>
+      <c r="S12" s="10">
+        <f t="shared" si="0"/>
         <v>-1.6945714285714286</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="6">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>-22.071999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>0.16</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>-6.0019999999999998</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>-0.47399999999999998</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <v>-4.8259999999999996</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="6">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="0"/>
+      <c r="I13" s="10">
+        <f t="shared" si="1"/>
         <v>-4.7412857142857145</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="6">
         <v>0.63400000000000001</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="6">
         <v>0.14499999999999999</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="6">
         <v>0.35799999999999998</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="6">
         <v>-1.056</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="6">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="6">
         <v>-6.5330000000000004</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="6">
         <v>0.80500000000000005</v>
       </c>
-      <c r="S13" s="3">
-        <f>AVERAGE(L13:R13)</f>
+      <c r="S13" s="10">
+        <f t="shared" si="0"/>
         <v>-0.70214285714285729</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <v>0.71</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>-3.0840000000000001</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>0.32200000000000001</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>-2.786</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>0.115</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <v>-3.9550000000000001</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>0.23400000000000001</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="0"/>
+      <c r="I14" s="10">
+        <f t="shared" si="1"/>
         <v>-1.2062857142857144</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <v>0.59599999999999997</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
         <v>-10.510999999999999</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="6">
         <v>0.34399999999999997</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="6">
         <v>0.23799999999999999</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="6">
         <v>0.435</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="6">
         <v>-0.248</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="S14" s="3">
-        <f>AVERAGE(L14:R14)</f>
+      <c r="S14" s="10">
+        <f t="shared" si="0"/>
         <v>-1.2234285714285711</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>0.755</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>-35.832999999999998</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>0.315</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>-15.010999999999999</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <v>0.27400000000000002</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <v>-15.532</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="6">
         <v>0.48199999999999998</v>
       </c>
-      <c r="I15" s="3">
-        <f t="shared" si="0"/>
+      <c r="I15" s="10">
+        <f t="shared" si="1"/>
         <v>-9.2214285714285715</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="6">
         <v>0.59199999999999997</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="6">
         <v>-0.60499999999999998</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="6">
         <v>0.153</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="6">
         <v>-1.746</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="6">
         <v>-0.24399999999999999</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="6">
         <v>-0.42699999999999999</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="6">
         <v>0.65900000000000003</v>
       </c>
-      <c r="S15" s="3">
-        <f>AVERAGE(L15:R15)</f>
+      <c r="S15" s="10">
+        <f t="shared" si="0"/>
         <v>-0.23114285714285715</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>0.48899999999999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>-59.792999999999999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>0.309</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>-620.23699999999997</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="6">
         <v>0.76</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <v>-15.16</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="6">
         <v>0.76300000000000001</v>
       </c>
-      <c r="I16" s="3">
-        <f t="shared" si="0"/>
+      <c r="I16" s="10">
+        <f t="shared" si="1"/>
         <v>-98.981285714285704</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="6">
         <v>0.58699999999999997</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="6">
         <v>-56.161999999999999</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="6">
         <v>0.41199999999999998</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="6">
         <v>-76.369</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="6">
         <v>0.17399999999999999</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="6">
         <v>0.32700000000000001</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="6">
         <v>0.56399999999999995</v>
       </c>
-      <c r="S16" s="3">
-        <f>AVERAGE(L16:R16)</f>
+      <c r="S16" s="10">
+        <f t="shared" si="0"/>
         <v>-18.638142857142856</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <v>0.59599999999999997</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>-10.510999999999999</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>0.34399999999999997</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>0.23799999999999999</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <v>0.435</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <v>-0.248</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="I17" s="3">
-        <f t="shared" si="0"/>
+      <c r="I17" s="10">
+        <f t="shared" si="1"/>
         <v>-1.2234285714285711</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="6">
         <v>0.55200000000000005</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="6">
         <v>-36.090000000000003</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="6">
         <v>0.39500000000000002</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="6">
         <v>-109.74299999999999</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="6">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="6">
         <v>-28.056000000000001</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="6">
         <v>0.4</v>
       </c>
-      <c r="S17" s="3">
-        <f>AVERAGE(L17:R17)</f>
+      <c r="S17" s="10">
+        <f t="shared" si="0"/>
         <v>-24.539571428571431</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>-1.123</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>-6.68</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <v>-1.909</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>-14.901</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="6">
         <v>0.46500000000000002</v>
       </c>
-      <c r="I18" s="3">
-        <f t="shared" si="0"/>
+      <c r="I18" s="10">
+        <f t="shared" si="1"/>
         <v>-3.3554285714285714</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="6">
         <v>0.52300000000000002</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="6">
         <v>-1.123</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="6">
         <v>0.13700000000000001</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="6">
         <v>-6.68</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="6">
         <v>-1.909</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="6">
         <v>-14.901</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="6">
         <v>0.46500000000000002</v>
       </c>
-      <c r="S18" s="3">
-        <f>AVERAGE(L18:R18)</f>
+      <c r="S18" s="10">
+        <f t="shared" si="0"/>
         <v>-3.3554285714285714</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>0.43099999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>-1.569</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>-2.7730000000000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <v>-0.58799999999999997</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="6">
         <v>-14.455</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="6">
         <v>0.28599999999999998</v>
       </c>
-      <c r="I19" s="3">
-        <f t="shared" si="0"/>
+      <c r="I19" s="10">
+        <f t="shared" si="1"/>
         <v>-2.6614285714285715</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="6">
         <v>0.502</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="6">
         <v>0.35899999999999999</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="6">
         <v>0.20599999999999999</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="6">
         <v>-11.425000000000001</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="6">
         <v>0.69299999999999995</v>
       </c>
-      <c r="S19" s="3">
-        <f>AVERAGE(L19:R19)</f>
+      <c r="S19" s="10">
+        <f t="shared" si="0"/>
         <v>-1.3277142857142861</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>-123.502</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>-250.1</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <v>-0.95699999999999996</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <v>-34.518999999999998</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="6">
         <v>0.65700000000000003</v>
       </c>
-      <c r="I20" s="3">
-        <f t="shared" si="0"/>
+      <c r="I20" s="10">
+        <f t="shared" si="1"/>
         <v>-58.205714285714286</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="6">
         <v>0.5</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="6">
         <v>-37.713999999999999</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="6">
         <v>0.189</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="6">
         <v>-0.51900000000000002</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="6">
         <v>0.24099999999999999</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="6">
         <v>-0.51800000000000002</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="6">
         <v>0.44500000000000001</v>
       </c>
-      <c r="S20" s="3">
-        <f>AVERAGE(L20:R20)</f>
+      <c r="S20" s="10">
+        <f t="shared" si="0"/>
         <v>-5.339428571428571</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>0.64100000000000001</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>0.40899999999999997</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>0.39100000000000001</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>-8.952</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="6">
         <v>0.124</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <v>-1.091</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="6">
         <v>0.71899999999999997</v>
       </c>
-      <c r="I21" s="3">
-        <f t="shared" si="0"/>
+      <c r="I21" s="10">
+        <f t="shared" si="1"/>
         <v>-1.1084285714285713</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="6">
         <v>0.48899999999999999</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="6">
         <v>-59.792999999999999</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="6">
         <v>0.309</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="6">
         <v>-620.23699999999997</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="6">
         <v>0.76</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="6">
         <v>-15.16</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="6">
         <v>0.76300000000000001</v>
       </c>
-      <c r="S21" s="3">
-        <f>AVERAGE(L21:R21)</f>
+      <c r="S21" s="10">
+        <f t="shared" si="0"/>
         <v>-98.981285714285704</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
         <v>0.115</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>-6.8540000000000001</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>0.21</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>-29.173999999999999</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="6">
         <v>-12.29</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I22" s="3">
-        <f t="shared" si="0"/>
+      <c r="I22" s="10">
+        <f t="shared" si="1"/>
         <v>-6.8415714285714282</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="6">
         <v>0.48899999999999999</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="6">
         <v>-30.119</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="6">
         <v>0.29899999999999999</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="6">
         <v>-123.947</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="6">
         <v>0.53600000000000003</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="6">
         <v>-32.948999999999998</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="S22" s="3">
-        <f>AVERAGE(L22:R22)</f>
+      <c r="S22" s="10">
+        <f t="shared" si="0"/>
         <v>-26.441142857142854</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>0.82599999999999996</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>-48.878</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>0.51900000000000002</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>-15.824999999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <v>0.85699999999999998</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <v>-16.427</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="6">
         <v>0.89600000000000002</v>
       </c>
-      <c r="I23" s="3">
-        <f t="shared" si="0"/>
+      <c r="I23" s="10">
+        <f t="shared" si="1"/>
         <v>-11.147428571428572</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="6">
         <v>0.43099999999999999</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="6">
         <v>-1.569</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="6">
         <v>-2.7730000000000001</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="6">
         <v>-0.58799999999999997</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="6">
         <v>-14.455</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="6">
         <v>0.28599999999999998</v>
       </c>
-      <c r="S23" s="3">
-        <f>AVERAGE(L23:R23)</f>
+      <c r="S23" s="10">
+        <f t="shared" si="0"/>
         <v>-2.6614285714285715</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="6">
         <v>0.59199999999999997</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>-0.60499999999999998</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>0.153</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <v>-1.746</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <v>-0.24399999999999999</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="6">
         <v>-0.42699999999999999</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="6">
         <v>0.65900000000000003</v>
       </c>
-      <c r="I24" s="3">
-        <f t="shared" si="0"/>
+      <c r="I24" s="10">
+        <f t="shared" si="1"/>
         <v>-0.23114285714285715</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="6">
         <v>0.34599999999999997</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="6">
         <v>-5.476</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="6">
         <v>-6.9000000000000006E-2</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="6">
         <v>-3.0419999999999998</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="6">
         <v>-1.0760000000000001</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="6">
         <v>-20.052</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="6">
         <v>0.16900000000000001</v>
       </c>
-      <c r="S24" s="3">
-        <f>AVERAGE(L24:R24)</f>
+      <c r="S24" s="10">
+        <f t="shared" si="0"/>
         <v>-4.1714285714285717</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="6">
         <v>0.55200000000000005</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>-36.090000000000003</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>0.39500000000000002</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>-109.74299999999999</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <v>0.76500000000000001</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <v>-28.056000000000001</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="6">
         <v>0.4</v>
       </c>
-      <c r="I25" s="3">
-        <f t="shared" si="0"/>
+      <c r="I25" s="10">
+        <f t="shared" si="1"/>
         <v>-24.539571428571431</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="6">
         <v>0.32</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="6">
         <v>-6.8029999999999999</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="6">
         <v>0.21199999999999999</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="6">
         <v>-1.0389999999999999</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="6">
         <v>0.23200000000000001</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="6">
         <v>-2.1989999999999998</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="6">
         <v>0.45500000000000002</v>
       </c>
-      <c r="S25" s="3">
-        <f>AVERAGE(L25:R25)</f>
+      <c r="S25" s="10">
+        <f t="shared" si="0"/>
         <v>-1.2602857142857142</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="6">
         <v>0.58699999999999997</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>-56.161999999999999</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>-76.369</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <v>0.17399999999999999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="6">
         <v>0.32700000000000001</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="6">
         <v>0.56399999999999995</v>
       </c>
-      <c r="I26" s="3">
-        <f t="shared" si="0"/>
+      <c r="I26" s="10">
+        <f t="shared" si="1"/>
         <v>-18.638142857142856</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="6">
         <v>0.158</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="6">
         <v>-1.5429999999999999</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="6">
         <v>-0.218</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="6">
         <v>-6.4180000000000001</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="6">
         <v>-0.187</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="6">
         <v>-7.1369999999999996</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="6">
         <v>-0.27300000000000002</v>
       </c>
-      <c r="S26" s="3">
-        <f>AVERAGE(L26:R26)</f>
+      <c r="S26" s="10">
+        <f t="shared" si="0"/>
         <v>-2.2311428571428569</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="6">
         <v>0.70399999999999996</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>-131.82499999999999</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>0.16400000000000001</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>-242.89599999999999</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <v>0.45200000000000001</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <v>-83.959000000000003</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="6">
         <v>0.61</v>
       </c>
-      <c r="I27" s="3">
-        <f t="shared" si="0"/>
+      <c r="I27" s="10">
+        <f t="shared" si="1"/>
         <v>-65.249999999999986</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="6">
         <v>0.15</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="6">
         <v>-6.9770000000000003</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="6">
         <v>0.30599999999999999</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="6">
         <v>-36.598999999999997</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="6">
         <v>0.372</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="6">
         <v>-14.78</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="6">
         <v>0.625</v>
       </c>
-      <c r="S27" s="3">
-        <f>AVERAGE(L27:R27)</f>
+      <c r="S27" s="10">
+        <f t="shared" si="0"/>
         <v>-8.1289999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="6">
         <v>0.105</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>-2.2679999999999998</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="6">
         <v>-5.9980000000000002</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="6">
         <v>-1.2809999999999999</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <v>-6.7439999999999998</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="6">
         <v>-0.623</v>
       </c>
-      <c r="I28" s="3">
-        <f t="shared" si="0"/>
+      <c r="I28" s="10">
+        <f t="shared" si="1"/>
         <v>-2.3939999999999997</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="6">
         <v>0.115</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="6">
         <v>-6.8540000000000001</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="6">
         <v>0.21</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="6">
         <v>-29.173999999999999</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="6">
         <v>-12.29</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="S28" s="3">
-        <f>AVERAGE(L28:R28)</f>
+      <c r="S28" s="10">
+        <f t="shared" si="0"/>
         <v>-6.8415714285714282</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="6">
         <v>0.64600000000000002</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>-2.1859999999999999</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>0.378</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>-4.718</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <v>0.47099999999999997</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <v>-1.0900000000000001</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="6">
         <v>0.78100000000000003</v>
       </c>
-      <c r="I29" s="3">
-        <f t="shared" si="0"/>
+      <c r="I29" s="10">
+        <f t="shared" si="1"/>
         <v>-0.81685714285714284</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="6">
         <v>0.105</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="6">
         <v>-2.2679999999999998</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="6">
         <v>-5.9980000000000002</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="6">
         <v>-1.2809999999999999</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="6">
         <v>-6.7439999999999998</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="6">
         <v>-0.623</v>
       </c>
-      <c r="S29" s="3">
-        <f>AVERAGE(L29:R29)</f>
+      <c r="S29" s="10">
+        <f t="shared" si="0"/>
         <v>-2.3939999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="6">
         <v>0.77400000000000002</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>-36.286999999999999</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>-5.8650000000000002</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="6">
         <v>-0.06</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="6">
         <v>-5.319</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="6">
         <v>0.23799999999999999</v>
       </c>
-      <c r="I30" s="3">
-        <f t="shared" si="0"/>
+      <c r="I30" s="10">
+        <f t="shared" si="1"/>
         <v>-6.6317142857142866</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="6">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="6">
         <v>-22.071999999999999</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="6">
         <v>0.16</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="6">
         <v>-6.0019999999999998</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="6">
         <v>-0.47399999999999998</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="6">
         <v>-4.8259999999999996</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="6">
         <v>0.23200000000000001</v>
       </c>
-      <c r="S30" s="3">
-        <f>AVERAGE(L30:R30)</f>
+      <c r="S30" s="10">
+        <f t="shared" si="0"/>
         <v>-4.7412857142857145</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="6">
         <v>0.48899999999999999</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>-30.119</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>0.29899999999999999</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="6">
         <v>-123.947</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="6">
         <v>0.53600000000000003</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
         <v>-32.948999999999998</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="I31" s="3">
-        <f t="shared" si="0"/>
+      <c r="I31" s="10">
+        <f t="shared" si="1"/>
         <v>-26.441142857142854</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="K31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="6">
         <v>-0.27600000000000002</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="6">
         <v>-3.2829999999999999</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="6">
         <v>-1392.027</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="6">
         <v>-13.678000000000001</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="6">
         <v>-1.044</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="6">
         <v>-3.8540000000000001</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="6">
         <v>-7.6820000000000004</v>
       </c>
-      <c r="S31" s="3">
-        <f>AVERAGE(L31:R31)</f>
+      <c r="S31" s="10">
+        <f t="shared" si="0"/>
         <v>-203.12057142857148</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="6">
         <v>0.83199999999999996</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>-48.353000000000002</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>0.44</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="6">
         <v>-34.415999999999997</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="6">
         <v>0.76500000000000001</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="6">
         <v>0.70299999999999996</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="6">
         <v>0.86299999999999999</v>
       </c>
-      <c r="I32" s="4">
-        <f t="shared" si="0"/>
+      <c r="I32" s="11">
+        <f t="shared" si="1"/>
         <v>-11.309428571428571</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="6">
         <v>-0.625</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="6">
         <v>-1.4890000000000001</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="6">
         <v>-0.20399999999999999</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="6">
         <v>-4.0170000000000003</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="6">
         <v>-0.75700000000000001</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="6">
         <v>-0.97699999999999998</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="6">
         <v>-0.32800000000000001</v>
       </c>
-      <c r="S32" s="4">
-        <f>AVERAGE(L32:R32)</f>
+      <c r="S32" s="11">
+        <f t="shared" si="0"/>
         <v>-1.1995714285714285</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K2:S32" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K3:S32">
-      <sortCondition descending="1" ref="L2:L32"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="L1:S1"/>

</xml_diff>